<commit_message>
manual testing - testcases and bug log updated
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amey/Documents/GitHub/project-g3t4/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A11B1DB-CF92-9640-BE5A-817C0AF877A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB268D9-D66D-4B42-AF52-E0FCBB68BB7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1 – Manual – Login Bo" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 1 - JSON - Login" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 1 – JSON – Authentica" sheetId="3" r:id="rId3"/>
+    <sheet name="Iteration 2 - Manual - Round 1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="232">
   <si>
     <t>S/N</t>
   </si>
@@ -985,12 +986,99 @@
   <si>
     <t xml:space="preserve">Bootstrap succeeded. </t>
   </si>
+  <si>
+    <t>In round 1, student can only bid for courses offered from their school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrapping includes a student from SOB bid in SIS </t>
+  </si>
+  <si>
+    <t>Perform bootstrapping which includes a bid from zac.ng(SOB student) for IS100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Not own school course " error </t>
+  </si>
+  <si>
+    <t>Bootstrap successful</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Manually bid for IS110 from a SOB student</t>
+  </si>
+  <si>
+    <t>"IS101 is not offered by your school" error</t>
+  </si>
+  <si>
+    <t>"IS100" is not offered by your school" error</t>
+  </si>
+  <si>
+    <t>zac.ng(SOB student) bids e$10 for IS100</t>
+  </si>
+  <si>
+    <t>In round 1, student can bid for courses offered from their school</t>
+  </si>
+  <si>
+    <t>Minimum of 10 e$ is required to bid for a course</t>
+  </si>
+  <si>
+    <t>Bid 5 e$ for a course</t>
+  </si>
+  <si>
+    <t>"A minimum bid for e$10 is required" error is popped up</t>
+  </si>
+  <si>
+    <t>You have succesfully bidded $5 for ECON001 S1</t>
+  </si>
+  <si>
+    <t>ursula.ng bids 5e$ for ECON001 S1</t>
+  </si>
+  <si>
+    <t>Prerequiste checking</t>
+  </si>
+  <si>
+    <t>ben.ng (has completed IS102.IS103) and is now bidding for IS104</t>
+  </si>
+  <si>
+    <t>bid IS104 S1 for e$10 via ben.ng account</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>amy.ng (has not completed IS103) and is now bidding for IS104</t>
+  </si>
+  <si>
+    <t>bid IS104 S1 for e$10 via amy.ng account</t>
+  </si>
+  <si>
+    <t>"You have not completed prerequisite course IS102"</t>
+  </si>
+  <si>
+    <t>ben.ng (has completed IS103 but not IS106) and is now bidding for IS203</t>
+  </si>
+  <si>
+    <t>bid IS203 S1 for e$10 via ben.ng account</t>
+  </si>
+  <si>
+    <t>"You have not completed prerequisite course IS106"</t>
+  </si>
+  <si>
+    <t>amy.ng (has not completed IS103, IS106) and is now bidding for IS104</t>
+  </si>
+  <si>
+    <t>bid IS203 S1 for e$10 via amy.ng account</t>
+  </si>
+  <si>
+    <t>"You have not completed prerequisite course IS103, You have not completed prerequisite course IS106"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1022,6 +1110,12 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1119,7 +1213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1143,6 +1237,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,8 +1461,8 @@
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="134" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2979,7 +3076,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3068,4 +3165,730 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03581E9B-5434-EB41-ABEB-2F66EF42EF28}">
+  <dimension ref="A1:H56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <cols>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="66" customHeight="1">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="63" customHeight="1">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="14">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="14">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="14">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="14">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="14">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="14">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="14">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="14">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" ht="14">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" ht="14">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="14">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="14">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" ht="14">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" ht="14">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="14">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="14">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" ht="14">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="14">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" ht="14">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="14">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" ht="14">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" ht="14">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="14">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" ht="14">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" ht="14">
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" ht="14">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" ht="14">
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" ht="14">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" ht="14">
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" ht="14">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" ht="14">
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" ht="14">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" ht="14">
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" ht="14">
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" ht="14">
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" ht="14">
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" ht="14">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" ht="14">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8" ht="14">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" ht="14">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" ht="14">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" ht="14">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" ht="14">
+      <c r="A54" s="4"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" ht="14">
+      <c r="A55" s="4"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="1:8" ht="14">
+      <c r="A56" s="4"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
JSON testcases updated in excel file
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rou Hui\Documents\GitHub\project-g3t4\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amey/Documents/GitHub/project-g3t4/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39E3E23-BA92-47E7-962C-53E42B62672D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3213DF3F-6A19-2545-A9E1-8E0E3EF25A9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1 – Manual – Login Bo" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 1 - JSON - Login" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 1 – JSON – Authentica" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration 2 - Manual - Round 1" sheetId="4" r:id="rId4"/>
-    <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId5"/>
+    <sheet name="Iteration 2 -- JSON" sheetId="6" r:id="rId5"/>
+    <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="351">
   <si>
     <t>S/N</t>
   </si>
@@ -1341,26 +1342,1010 @@
     <t>student bids for section that has 0 vancancies with the minimum bid</t>
   </si>
   <si>
-    <t xml:space="preserve">ben.ong bids e$12 for IS100 </t>
-  </si>
-  <si>
     <t>"Pending, fail"</t>
   </si>
   <si>
     <t>student bids for section that has vacancies with the minimum bid</t>
   </si>
   <si>
-    <t>ben.ong bids for e$14.01 for IS100</t>
-  </si>
-  <si>
     <t>"Pending, successful"</t>
+  </si>
+  <si>
+    <t>ben.ng bids for e$14.01 for IS100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ben.ng bids e$12 for IS100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 students bid the same amount for one vacancy </t>
+  </si>
+  <si>
+    <t>ben.ng and za.ng bid e$10 for is100</t>
+  </si>
+  <si>
+    <t>both unsucessful</t>
+  </si>
+  <si>
+    <t>error thrown</t>
+  </si>
+  <si>
+    <t>username=calvin.ng.2009</t>
+  </si>
+  <si>
+    <t>username=calvin.ng.2009
+password=qwerty130</t>
+  </si>
+  <si>
+    <t>username=calvin.ng.2009
+password=wrongpasswordhaha</t>
+  </si>
+  <si>
+    <t>EMPTY</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS102","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "ada.goh.2012","amount": 11.0,"course": "IS100","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","amount": 9.0,"course": "IS100","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS110","section": "S1"}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "round not started"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "round": "1"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "courses": [
+        {
+            "course": "ECON001",
+            "school": "SOE",
+            "title": "Microeconomics",
+            "description": "Microeconomics is about economics in smaller scale (e.g. firm-scale)",
+            "examdate": "20131101",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "ECON002",
+            "school": "SOE",
+            "title": "Macroeconomics",
+            "description": "You don't learn about excel macros here.",
+            "examdate": "20131101",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS100",
+            "school": "SIS",
+            "title": "Calculus ",
+            "description": "The basic objective of Calculus is to relate small-scale (differential) quantities to large-scale (integrated) quantities. This is accomplished by means of the Fundamental Theorem of Calculus. Students should demonstrate an understanding of the integral as a cumulative sum, of the derivative as a rate of change, and of the inverse relationship between integration and differentiation.",
+            "examdate": "20131119",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS101",
+            "school": "SIS",
+            "title": "Advanced Calculus",
+            "description": "This is a second course on calculus.\u00a0It is more advanced definitely.",
+            "examdate": "20131118",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS102",
+            "school": "SIS",
+            "title": "Java programming",
+            "description": "This course teaches you on Java programming. I love Java definitely.",
+            "examdate": "20131117",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS103",
+            "school": "SIS",
+            "title": "Web Programming",
+            "description": "JSP, Servlets using Tomcat",
+            "examdate": "20131116",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS104",
+            "school": "SIS",
+            "title": "Advanced Programming",
+            "description": "How to write code that nobody can understand",
+            "examdate": "20131115",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS105",
+            "school": "SIS",
+            "title": "Data Structures",
+            "description": "Data structure is a particular way of storing and organizing data in a computer so that it can be used efficiently. Arrays, Lists, Stacks and Trees will be covered.",
+            "examdate": "20131114",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS106",
+            "school": "SIS",
+            "title": "Database Modeling &amp; Design",
+            "description": "Data modeling in software engineering is the process of creating a data model by applying formal data model descriptions using data modeling techniques. ",
+            "examdate": "20131113",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS107",
+            "school": "SIS",
+            "title": "IT Outsourcing",
+            "description": "This course teaches you on how to outsource your programming projects to others.",
+            "examdate": "20131112",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS108",
+            "school": "SIS",
+            "title": "Organization Behaviour",
+            "description": "Organizational Behavior (OB) is the study and application of knowledge about how people, individuals, and groups act in organizations. ",
+            "examdate": "20131111",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS109",
+            "school": "SIS",
+            "title": "Cloud Computing",
+            "description": "Cloud computing is Internet-based computing, whereby shared resources, software and information are provided to computers and other devices on-demand, like the electricity grid.",
+            "examdate": "20131110",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS200",
+            "school": "SIS",
+            "title": "Final Touch",
+            "description": "Learn how eat, dress and talk.",
+            "examdate": "20131109",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS201",
+            "school": "SIS",
+            "title": "Fun with Shell Programming",
+            "description": "Shell scripts are a fundamental part of the UNIX and Linux programming environment.",
+            "examdate": "20131108",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS202",
+            "school": "SIS",
+            "title": "Enterprise integration",
+            "description": "Enterprise integration is a technical field of Enterprise Architecture, which focused on the study of things like system interconnection, electronic data interchange, product data exchange and distributed computing environments, and it's possible other solutions.[1",
+            "examdate": "20131107",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS203",
+            "school": "SIS",
+            "title": "Software Engineering",
+            "description": "The Sleepless Era.",
+            "examdate": "20131106",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS204",
+            "school": "SIS",
+            "title": "Database System Administration",
+            "description": "Database administration is a complex, often thankless chore.",
+            "examdate": "20131105",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS205",
+            "school": "SIS",
+            "title": "All Talk, No Action",
+            "description": "The easiest course of all. We will sit around and talk.",
+            "examdate": "20131104",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS206",
+            "school": "SIS",
+            "title": "Operation Research",
+            "description": "Operations research, also known as operational research, is an interdisciplinary branch of applied mathematics and formal science that uses advanced analytical methods such as mathematical modeling, statistical analysis, and mathematical optimization to arrive at optimal or near-optimal solutions to complex decision-making problems.",
+            "examdate": "20131103",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS207",
+            "school": "SIS",
+            "title": "GUI Bloopers",
+            "description": "Common User Interface Design Don'ts and Dos",
+            "examdate": "20131103",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS208",
+            "school": "SIS",
+            "title": "Artifical Intelligence",
+            "description": "The science and engineering of making intelligent machine",
+            "examdate": "20131103",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS209",
+            "school": "SIS",
+            "title": "Information Storage and Management",
+            "description": "Information storage and management (ISM) - once a relatively straightforward operation -has developed into a highly sophisticated pillar of information technology, requiring proven technical expertise.",
+            "examdate": "20131102",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "MGMT001",
+            "school": "SOB",
+            "title": "Business,Government, and Society",
+            "description": "learn the interrelation amongst the three",
+            "examdate": "20131102",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "MGMT002",
+            "school": "SOB",
+            "title": "Technology and World Change",
+            "description": "As technology changes, so does the world",
+            "examdate": "20131101",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        }
+    ],
+    "section": [
+        {
+            "course": "ECON001",
+            "section": "S1",
+            "day": "4",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "John KHOO",
+            "venue": "Seminar Rm 2-34",
+            "size": "10"
+        },
+        {
+            "course": "ECON002",
+            "section": "S1",
+            "day": "5",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Andy KHOO",
+            "venue": "Seminar Rm 2-35",
+            "size": "10"
+        },
+        {
+            "course": "IS100",
+            "section": "S1",
+            "day": "1",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Albert KHOO",
+            "venue": "Seminar Rm 2-1",
+            "size": "10"
+        },
+        {
+            "course": "IS100",
+            "section": "S2",
+            "day": "2",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Billy KHOO",
+            "venue": "Seminar Rm 2-2",
+            "size": "10"
+        },
+        {
+            "course": "IS101",
+            "section": "S1",
+            "day": "3",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Cheri KHOO",
+            "venue": "Seminar Rm 2-3",
+            "size": "10"
+        },
+        {
+            "course": "IS101",
+            "section": "S2",
+            "day": "4",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Daniel KHOO",
+            "venue": "Seminar Rm 2-4",
+            "size": "10"
+        },
+        {
+            "course": "IS101",
+            "section": "S3",
+            "day": "5",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Ernest KHOO",
+            "venue": "Seminar Rm 2-5",
+            "size": "10"
+        },
+        {
+            "course": "IS102",
+            "section": "S1",
+            "day": "1",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Felicia KHOO",
+            "venue": "Seminar Rm 2-6",
+            "size": "10"
+        },
+        {
+            "course": "IS102",
+            "section": "S2",
+            "day": "2",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Gerald KHOO",
+            "venue": "Seminar Rm 2-7",
+            "size": "10"
+        },
+        {
+            "course": "IS102",
+            "section": "S3",
+            "day": "3",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Henry KHOO",
+            "venue": "Seminar Rm 2-8",
+            "size": "10"
+        },
+        {
+            "course": "IS103",
+            "section": "S1",
+            "day": "4",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Ivy KHOO",
+            "venue": "Seminar Rm 2-9",
+            "size": "10"
+        },
+        {
+            "course": "IS103",
+            "section": "S2",
+            "day": "5",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Jason KHOO",
+            "venue": "Seminar Rm 2-10",
+            "size": "10"
+        },
+        {
+            "course": "IS103",
+            "section": "S3",
+            "day": "1",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Kat KHOO",
+            "venue": "Seminar Rm 2-11",
+            "size": "10"
+        },
+        {
+            "course": "IS104",
+            "section": "S1",
+            "day": "2",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Linn KHOO",
+            "venue": "Seminar Rm 2-12",
+            "size": "10"
+        },
+        {
+            "course": "IS104",
+            "section": "S2",
+            "day": "3",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Michael KHOO",
+            "venue": "Seminar Rm 2-13",
+            "size": "10"
+        },
+        {
+            "course": "IS105",
+            "section": "S1",
+            "day": "4",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Nathaniel KHOO",
+            "venue": "Seminar Rm 2-14",
+            "size": "10"
+        },
+        {
+            "course": "IS105",
+            "section": "S2",
+            "day": "5",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Oreilly KHOO",
+            "venue": "Seminar Rm 2-15",
+            "size": "10"
+        },
+        {
+            "course": "IS106",
+            "section": "S1",
+            "day": "1",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Peter KHOO",
+            "venue": "Seminar Rm 2-16",
+            "size": "10"
+        },
+        {
+            "course": "IS106",
+            "section": "S2",
+            "day": "2",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Queen KHOO",
+            "venue": "Seminar Rm 2-17",
+            "size": "10"
+        },
+        {
+            "course": "IS107",
+            "section": "S1",
+            "day": "3",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Ray KHOO",
+            "venue": "Seminar Rm 2-18",
+            "size": "10"
+        },
+        {
+            "course": "IS107",
+            "section": "S2",
+            "day": "4",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Simon KHOO",
+            "venue": "Seminar Rm 2-19",
+            "size": "10"
+        },
+        {
+            "course": "IS108",
+            "section": "S1",
+            "day": "5",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Tim KHOO",
+            "venue": "Seminar Rm 2-20",
+            "size": "10"
+        },
+        {
+            "course": "IS109",
+            "section": "S1",
+            "day": "2",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Vincent KHOO",
+            "venue": "Seminar Rm 2-22",
+            "size": "10"
+        },
+        {
+            "course": "IS109",
+            "section": "S2",
+            "day": "3",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Winnie KHOO",
+            "venue": "Seminar Rm 2-23",
+            "size": "10"
+        },
+        {
+            "course": "IS200",
+            "section": "S1",
+            "day": "4",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Xtra KHOO",
+            "venue": "Seminar Rm 2-24",
+            "size": "10"
+        },
+        {
+            "course": "IS201",
+            "section": "S1",
+            "day": "5",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Yale KHOO",
+            "venue": "Seminar Rm 2-25",
+            "size": "10"
+        },
+        {
+            "course": "IS202",
+            "section": "S1",
+            "day": "1",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Zen KHOO",
+            "venue": "Seminar Rm 2-26",
+            "size": "10"
+        },
+        {
+            "course": "IS203",
+            "section": "S1",
+            "day": "2",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Anderson KHOO",
+            "venue": "Seminar Rm 2-27",
+            "size": "10"
+        },
+        {
+            "course": "IS204",
+            "section": "S1",
+            "day": "3",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Bing KHOO",
+            "venue": "Seminar Rm 2-28",
+            "size": "10"
+        },
+        {
+            "course": "IS205",
+            "section": "S1",
+            "day": "4",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Carlo KHOO",
+            "venue": "Seminar Rm 2-29",
+            "size": "10"
+        },
+        {
+            "course": "IS206",
+            "section": "S1",
+            "day": "5",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Dickson KHOO",
+            "venue": "Seminar Rm 2-30",
+            "size": "10"
+        },
+        {
+            "course": "IS207",
+            "section": "S1",
+            "day": "1",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Edmund KHOO",
+            "venue": "Seminar Rm 2-31",
+            "size": "10"
+        },
+        {
+            "course": "IS208",
+            "section": "S1",
+            "day": "2",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Febrice KHOO",
+            "venue": "Seminar Rm 2-32",
+            "size": "10"
+        },
+        {
+            "course": "MGMT001",
+            "section": "S1",
+            "day": "3",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Gavin KHOO",
+            "venue": "Seminar Rm 2-33",
+            "size": "10"
+        },
+        {
+            "course": "MGMT002",
+            "section": "S1",
+            "day": "3",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Bob KHOO",
+            "venue": "Seminar Rm 2-37",
+            "size": "10"
+        }
+    ],
+    "students": [
+        {
+            "userid": "amy.ng.2009",
+            "password": "qwerty128",
+            "name": "Amy NG",
+            "school": "SIS",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "password": "qwerty129",
+            "name": "Ben NG",
+            "school": "SIS",
+            "edollar": "189.00"
+        },
+        {
+            "userid": "calvin.ng.2009",
+            "password": "qwerty130",
+            "name": "Calvin NG",
+            "school": "SIS",
+            "edollar": "188.00"
+        },
+        {
+            "userid": "dawn.ng.2009",
+            "password": "qwerty131",
+            "name": "Dawn NG",
+            "school": "SIS",
+            "edollar": "187.00"
+        },
+        {
+            "userid": "eddy.ng.2009",
+            "password": "qwerty132",
+            "name": "Eddy NG",
+            "school": "SIS",
+            "edollar": "186.00"
+        },
+        {
+            "userid": "fred.ng.2009",
+            "password": "qwerty133",
+            "name": "Fred NG",
+            "school": "SIS",
+            "edollar": "185.00"
+        },
+        {
+            "userid": "gary.ng.2009",
+            "password": "qwerty134",
+            "name": "Gary NG",
+            "school": "SIS",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "harry.ng.2009",
+            "password": "qwerty135",
+            "name": "Harry NG",
+            "school": "SIS",
+            "edollar": "183.00"
+        },
+        {
+            "userid": "ian.ng.2009",
+            "password": "qwerty136",
+            "name": "Ian NG",
+            "school": "SIS",
+            "edollar": "182.00"
+        },
+        {
+            "userid": "jerry.ng.2009",
+            "password": "qwerty137",
+            "name": "Jerry NG",
+            "school": "SIS",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "kelly.ng.2009",
+            "password": "qwerty138",
+            "name": "Kelly NG",
+            "school": "SIS",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "larry.ng.2009",
+            "password": "qwerty139",
+            "name": "Larry NG",
+            "school": "SIS",
+            "edollar": "181.00"
+        },
+        {
+            "userid": "maggie.ng.2009",
+            "password": "qwerty140",
+            "name": "Maggie NG",
+            "school": "SIS",
+            "edollar": "180.00"
+        },
+        {
+            "userid": "neilson.ng.2009",
+            "password": "qwerty141",
+            "name": "Neilson NG",
+            "school": "SIS",
+            "edollar": "179.00"
+        },
+        {
+            "userid": "olivia.ng.2009",
+            "password": "qwerty142",
+            "name": "Olivia NG",
+            "school": "SIS",
+            "edollar": "178.00"
+        },
+        {
+            "userid": "parker.ng.2009",
+            "password": "qwerty143",
+            "name": "Parker NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "quiten.ng.2009",
+            "password": "qwerty144",
+            "name": "Quiten NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "ricky.ng.2009",
+            "password": "qwerty145",
+            "name": "Ricky NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "steven.ng.2009",
+            "password": "qwerty146",
+            "name": "Steven NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "timothy.ng.2009",
+            "password": "qwerty147",
+            "name": "Timothy NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "ursala.ng.2009",
+            "password": "qwerty148",
+            "name": "Ursala NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "valarie.ng.2009",
+            "password": "qwerty149",
+            "name": "Valarie NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "winston.ng.2009",
+            "password": "qwerty150",
+            "name": "Winston NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "xavier.ng.2009",
+            "password": "qwerty151",
+            "name": "Xavier NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "yasir.ng.2009",
+            "password": "qwerty152",
+            "name": "Yasir NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "zac.ng.2009",
+            "password": "qwerty153",
+            "name": "Zac NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        }
+    ],
+    "prerequisite": [
+        {
+            "course": "IS101",
+            "prerequisite": "IS100"
+        },
+        {
+            "course": "IS103",
+            "prerequisite": "IS102"
+        },
+        {
+            "course": "IS104",
+            "prerequisite": "IS103"
+        },
+        {
+            "course": "IS109",
+            "prerequisite": "IS102"
+        },
+        {
+            "course": "IS203",
+            "prerequisite": "IS103"
+        },
+        {
+            "course": "IS203",
+            "prerequisite": "IS106"
+        },
+        {
+            "course": "IS204",
+            "prerequisite": "IS106"
+        },
+        {
+            "course": "IS209",
+            "prerequisite": "IS106"
+        }
+    ],
+    "bid": [
+        {
+            "userid": "olivia.ng.2009",
+            "amount": "22.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "neilson.ng.2009",
+            "amount": "21.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "maggie.ng.2009",
+            "amount": "20.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "larry.ng.2009",
+            "amount": "19.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "ian.ng.2009",
+            "amount": "18.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "harry.ng.2009",
+            "amount": "17.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "fred.ng.2009",
+            "amount": "15.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "eddy.ng.2009",
+            "amount": "14.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "dawn.ng.2009",
+            "amount": "13.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "calvin.ng.2009",
+            "amount": "12.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "amount": "11.00",
+            "course": "IS100",
+            "section": "S1"
+        }
+    ],
+    "completed-course": [
+        {
+            "userid": "amy.ng.2009",
+            "course": "IS100"
+        },
+        {
+            "userid": "gary.ng.2009",
+            "course": "IS100"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "course": "IS102"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "course": "IS103"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid userid"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Stop round</t>
+  </si>
+  <si>
+    <t>Start round</t>
+  </si>
+  <si>
+    <t>Dump</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid amount"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid course"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Update bid - succesful case</t>
+  </si>
+  <si>
+    <t>Update bid - enter invalid user</t>
+  </si>
+  <si>
+    <t>Update bid - enter invalid amount</t>
+  </si>
+  <si>
+    <t>Update bid - enter invalid course</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1750,16 +2735,16 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +2770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1795,7 +2780,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1821,7 +2806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="75">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1847,7 +2832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1873,7 +2858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="60">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1899,7 +2884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1925,7 +2910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1951,7 +2936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1977,7 +2962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="60">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2003,7 +2988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2029,7 +3014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2055,7 +3040,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2081,7 +3066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="120">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2107,7 +3092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="120">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2133,7 +3118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2159,7 +3144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2185,7 +3170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="45">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2211,7 +3196,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="75">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2237,7 +3222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="45">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2263,7 +3248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="120">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2289,7 +3274,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="45">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2315,7 +3300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="45">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2341,7 +3326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2367,7 +3352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="45">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2393,7 +3378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -2419,7 +3404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="60">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -2445,7 +3430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="45">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -2471,7 +3456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="98" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="105">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -2497,7 +3482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="409.6">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -2523,7 +3508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="224" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="225">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -2549,7 +3534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="45">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -2575,7 +3560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="45">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2601,7 +3586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="45">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -2627,7 +3612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="45">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -2653,7 +3638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="45">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -2679,7 +3664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="45">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -2705,7 +3690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="60">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -2731,7 +3716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="45">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -2757,7 +3742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="105">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -2783,7 +3768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="98" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="105">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -2809,7 +3794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="45">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -2835,7 +3820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="45">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -2861,7 +3846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="154" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="165">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -2887,7 +3872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="60">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -2913,7 +3898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="60">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -2939,7 +3924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="45">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -2965,7 +3950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="60">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -2991,7 +3976,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="60">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -3017,7 +4002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="45">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -3043,7 +4028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="45">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -3069,7 +4054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="45">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -3095,7 +4080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="45">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -3121,7 +4106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="45">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -3147,7 +4132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="60">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -3173,7 +4158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="60">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -3221,20 +4206,20 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView zoomScale="111" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="32.453125" customWidth="1"/>
-    <col min="4" max="4" width="78.453125" customWidth="1"/>
-    <col min="5" max="5" width="78.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="78.5" customWidth="1"/>
+    <col min="5" max="5" width="78.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +4239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="51.75" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -3262,7 +4247,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="98" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="105">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3282,7 +4267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3302,7 +4287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -3322,7 +4307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="60">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -3363,17 +4348,17 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6328125" customWidth="1"/>
-    <col min="5" max="5" width="32.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3393,7 +4378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="48" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -3401,7 +4386,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="168" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="180">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -3421,7 +4406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="409.6">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -3462,16 +4447,16 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
   <cols>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3497,7 +4482,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3507,7 +4492,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="66" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3533,7 +4518,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="63" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3559,7 +4544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3585,7 +4570,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3611,7 +4596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3637,7 +4622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3663,7 +4648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="60">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3689,7 +4674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3715,7 +4700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3741,7 +4726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3767,7 +4752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3793,7 +4778,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3819,7 +4804,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3845,7 +4830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="75">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3871,7 +4856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="75">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3897,7 +4882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="45">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3923,7 +4908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="45">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3949,7 +4934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="60">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3975,7 +4960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="45">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4001,7 +4986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="45">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4027,7 +5012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="75">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4053,7 +5038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -4079,7 +5064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4089,7 +5074,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="14">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4099,7 +5084,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4109,7 +5094,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4119,7 +5104,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4129,7 +5114,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4139,7 +5124,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4149,7 +5134,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4159,7 +5144,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="14">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4169,7 +5154,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="14">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4179,7 +5164,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="14">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4189,7 +5174,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="14">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4199,7 +5184,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="14">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4209,7 +5194,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4219,7 +5204,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="14">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4229,7 +5214,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="14">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4239,7 +5224,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="14">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -4249,7 +5234,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="14">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -4259,7 +5244,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="14">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -4269,7 +5254,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="14">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -4279,7 +5264,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="14">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -4289,7 +5274,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="14">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -4299,7 +5284,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="14">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -4309,7 +5294,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="14">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -4319,7 +5304,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="14">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4329,7 +5314,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="14">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -4339,7 +5324,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="14">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -4349,7 +5334,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="14">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -4359,7 +5344,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="14">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -4369,7 +5354,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="14">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -4379,7 +5364,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="14">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4389,7 +5374,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="14">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
@@ -4415,23 +5400,395 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED20DAA-AFB2-5240-A261-8BB8E5918D09}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <cols>
+    <col min="3" max="3" width="30.1640625" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="48" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="150">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="64" customHeight="1">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="77" customHeight="1">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="409.6">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="52" customHeight="1">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="90">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="14">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="14">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="14">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="14">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA8D5A-5628-41F0-8C3D-F219DADB62EC}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="C7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
   <cols>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4457,7 +5814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -4467,7 +5824,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="66" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4493,7 +5850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="63" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4519,7 +5876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4545,7 +5902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="75">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4571,7 +5928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="75">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4597,7 +5954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="90">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4623,7 +5980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="60">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4649,7 +6006,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4663,19 +6020,19 @@
         <v>318</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4686,32 +6043,48 @@
         <v>317</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>322</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -4721,7 +6094,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -4731,7 +6104,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="14">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4741,7 +6114,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
@@ -4751,7 +6124,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="14">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
@@ -4761,7 +6134,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="14">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4771,7 +6144,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="14">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4781,7 +6154,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="14">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4791,7 +6164,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="14">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4801,7 +6174,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="14">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4811,7 +6184,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="14">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4821,7 +6194,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="14">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4831,7 +6204,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4841,7 +6214,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="14">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4851,7 +6224,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4861,7 +6234,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4871,7 +6244,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4881,7 +6254,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4891,7 +6264,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4901,7 +6274,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4911,7 +6284,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="14">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4921,7 +6294,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="14">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4931,7 +6304,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="14">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4941,7 +6314,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="14">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4951,7 +6324,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="14">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4961,7 +6334,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4971,7 +6344,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="14">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4981,7 +6354,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="14">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4991,7 +6364,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="14">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5001,7 +6374,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="14">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5011,7 +6384,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="14">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -5021,7 +6394,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="14">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -5031,7 +6404,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="14">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -5041,7 +6414,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="14">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -5051,7 +6424,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="14">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -5061,7 +6434,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="14">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -5071,7 +6444,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="14">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -5081,7 +6454,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="14">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -5091,7 +6464,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="14">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5101,7 +6474,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="14">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5111,7 +6484,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="14">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -5121,7 +6494,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="14">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -5131,7 +6504,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="14">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -5141,7 +6514,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="14">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>

</xml_diff>

<commit_message>
Revert "JSON testcases updated in excel file"
This reverts commit 8f902bf73c8f1250231e61dfdde625056c23fc2c.
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amey/Documents/GitHub/project-g3t4/testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rou Hui\Documents\GitHub\project-g3t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3213DF3F-6A19-2545-A9E1-8E0E3EF25A9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39E3E23-BA92-47E7-962C-53E42B62672D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1 – Manual – Login Bo" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 1 - JSON - Login" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 1 – JSON – Authentica" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration 2 - Manual - Round 1" sheetId="4" r:id="rId4"/>
-    <sheet name="Iteration 2 -- JSON" sheetId="6" r:id="rId5"/>
-    <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId6"/>
+    <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="324">
   <si>
     <t>S/N</t>
   </si>
@@ -1342,1010 +1341,26 @@
     <t>student bids for section that has 0 vancancies with the minimum bid</t>
   </si>
   <si>
+    <t xml:space="preserve">ben.ong bids e$12 for IS100 </t>
+  </si>
+  <si>
     <t>"Pending, fail"</t>
   </si>
   <si>
     <t>student bids for section that has vacancies with the minimum bid</t>
   </si>
   <si>
+    <t>ben.ong bids for e$14.01 for IS100</t>
+  </si>
+  <si>
     <t>"Pending, successful"</t>
-  </si>
-  <si>
-    <t>ben.ng bids for e$14.01 for IS100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ben.ng bids e$12 for IS100 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 students bid the same amount for one vacancy </t>
-  </si>
-  <si>
-    <t>ben.ng and za.ng bid e$10 for is100</t>
-  </si>
-  <si>
-    <t>both unsucessful</t>
-  </si>
-  <si>
-    <t>error thrown</t>
-  </si>
-  <si>
-    <t>username=calvin.ng.2009</t>
-  </si>
-  <si>
-    <t>username=calvin.ng.2009
-password=qwerty130</t>
-  </si>
-  <si>
-    <t>username=calvin.ng.2009
-password=wrongpasswordhaha</t>
-  </si>
-  <si>
-    <t>EMPTY</t>
-  </si>
-  <si>
-    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS102","section": "S1"}</t>
-  </si>
-  <si>
-    <t>r={"userid": "ada.goh.2012","amount": 11.0,"course": "IS100","section": "S1"}</t>
-  </si>
-  <si>
-    <t>r={"userid": "amy.ng.2009","amount": 9.0,"course": "IS100","section": "S1"}</t>
-  </si>
-  <si>
-    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS110","section": "S1"}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "error",
-    "message": [
-        "round not started"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success",
-    "round": "1"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success",
-    "courses": [
-        {
-            "course": "ECON001",
-            "school": "SOE",
-            "title": "Microeconomics",
-            "description": "Microeconomics is about economics in smaller scale (e.g. firm-scale)",
-            "examdate": "20131101",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "ECON002",
-            "school": "SOE",
-            "title": "Macroeconomics",
-            "description": "You don't learn about excel macros here.",
-            "examdate": "20131101",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS100",
-            "school": "SIS",
-            "title": "Calculus ",
-            "description": "The basic objective of Calculus is to relate small-scale (differential) quantities to large-scale (integrated) quantities. This is accomplished by means of the Fundamental Theorem of Calculus. Students should demonstrate an understanding of the integral as a cumulative sum, of the derivative as a rate of change, and of the inverse relationship between integration and differentiation.",
-            "examdate": "20131119",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS101",
-            "school": "SIS",
-            "title": "Advanced Calculus",
-            "description": "This is a second course on calculus.\u00a0It is more advanced definitely.",
-            "examdate": "20131118",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS102",
-            "school": "SIS",
-            "title": "Java programming",
-            "description": "This course teaches you on Java programming. I love Java definitely.",
-            "examdate": "20131117",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS103",
-            "school": "SIS",
-            "title": "Web Programming",
-            "description": "JSP, Servlets using Tomcat",
-            "examdate": "20131116",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS104",
-            "school": "SIS",
-            "title": "Advanced Programming",
-            "description": "How to write code that nobody can understand",
-            "examdate": "20131115",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS105",
-            "school": "SIS",
-            "title": "Data Structures",
-            "description": "Data structure is a particular way of storing and organizing data in a computer so that it can be used efficiently. Arrays, Lists, Stacks and Trees will be covered.",
-            "examdate": "20131114",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS106",
-            "school": "SIS",
-            "title": "Database Modeling &amp; Design",
-            "description": "Data modeling in software engineering is the process of creating a data model by applying formal data model descriptions using data modeling techniques. ",
-            "examdate": "20131113",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS107",
-            "school": "SIS",
-            "title": "IT Outsourcing",
-            "description": "This course teaches you on how to outsource your programming projects to others.",
-            "examdate": "20131112",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS108",
-            "school": "SIS",
-            "title": "Organization Behaviour",
-            "description": "Organizational Behavior (OB) is the study and application of knowledge about how people, individuals, and groups act in organizations. ",
-            "examdate": "20131111",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS109",
-            "school": "SIS",
-            "title": "Cloud Computing",
-            "description": "Cloud computing is Internet-based computing, whereby shared resources, software and information are provided to computers and other devices on-demand, like the electricity grid.",
-            "examdate": "20131110",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS200",
-            "school": "SIS",
-            "title": "Final Touch",
-            "description": "Learn how eat, dress and talk.",
-            "examdate": "20131109",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS201",
-            "school": "SIS",
-            "title": "Fun with Shell Programming",
-            "description": "Shell scripts are a fundamental part of the UNIX and Linux programming environment.",
-            "examdate": "20131108",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS202",
-            "school": "SIS",
-            "title": "Enterprise integration",
-            "description": "Enterprise integration is a technical field of Enterprise Architecture, which focused on the study of things like system interconnection, electronic data interchange, product data exchange and distributed computing environments, and it's possible other solutions.[1",
-            "examdate": "20131107",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS203",
-            "school": "SIS",
-            "title": "Software Engineering",
-            "description": "The Sleepless Era.",
-            "examdate": "20131106",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS204",
-            "school": "SIS",
-            "title": "Database System Administration",
-            "description": "Database administration is a complex, often thankless chore.",
-            "examdate": "20131105",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS205",
-            "school": "SIS",
-            "title": "All Talk, No Action",
-            "description": "The easiest course of all. We will sit around and talk.",
-            "examdate": "20131104",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS206",
-            "school": "SIS",
-            "title": "Operation Research",
-            "description": "Operations research, also known as operational research, is an interdisciplinary branch of applied mathematics and formal science that uses advanced analytical methods such as mathematical modeling, statistical analysis, and mathematical optimization to arrive at optimal or near-optimal solutions to complex decision-making problems.",
-            "examdate": "20131103",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS207",
-            "school": "SIS",
-            "title": "GUI Bloopers",
-            "description": "Common User Interface Design Don'ts and Dos",
-            "examdate": "20131103",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS208",
-            "school": "SIS",
-            "title": "Artifical Intelligence",
-            "description": "The science and engineering of making intelligent machine",
-            "examdate": "20131103",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS209",
-            "school": "SIS",
-            "title": "Information Storage and Management",
-            "description": "Information storage and management (ISM) - once a relatively straightforward operation -has developed into a highly sophisticated pillar of information technology, requiring proven technical expertise.",
-            "examdate": "20131102",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "MGMT001",
-            "school": "SOB",
-            "title": "Business,Government, and Society",
-            "description": "learn the interrelation amongst the three",
-            "examdate": "20131102",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "MGMT002",
-            "school": "SOB",
-            "title": "Technology and World Change",
-            "description": "As technology changes, so does the world",
-            "examdate": "20131101",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        }
-    ],
-    "section": [
-        {
-            "course": "ECON001",
-            "section": "S1",
-            "day": "4",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "John KHOO",
-            "venue": "Seminar Rm 2-34",
-            "size": "10"
-        },
-        {
-            "course": "ECON002",
-            "section": "S1",
-            "day": "5",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Andy KHOO",
-            "venue": "Seminar Rm 2-35",
-            "size": "10"
-        },
-        {
-            "course": "IS100",
-            "section": "S1",
-            "day": "1",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Albert KHOO",
-            "venue": "Seminar Rm 2-1",
-            "size": "10"
-        },
-        {
-            "course": "IS100",
-            "section": "S2",
-            "day": "2",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Billy KHOO",
-            "venue": "Seminar Rm 2-2",
-            "size": "10"
-        },
-        {
-            "course": "IS101",
-            "section": "S1",
-            "day": "3",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Cheri KHOO",
-            "venue": "Seminar Rm 2-3",
-            "size": "10"
-        },
-        {
-            "course": "IS101",
-            "section": "S2",
-            "day": "4",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Daniel KHOO",
-            "venue": "Seminar Rm 2-4",
-            "size": "10"
-        },
-        {
-            "course": "IS101",
-            "section": "S3",
-            "day": "5",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Ernest KHOO",
-            "venue": "Seminar Rm 2-5",
-            "size": "10"
-        },
-        {
-            "course": "IS102",
-            "section": "S1",
-            "day": "1",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Felicia KHOO",
-            "venue": "Seminar Rm 2-6",
-            "size": "10"
-        },
-        {
-            "course": "IS102",
-            "section": "S2",
-            "day": "2",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Gerald KHOO",
-            "venue": "Seminar Rm 2-7",
-            "size": "10"
-        },
-        {
-            "course": "IS102",
-            "section": "S3",
-            "day": "3",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Henry KHOO",
-            "venue": "Seminar Rm 2-8",
-            "size": "10"
-        },
-        {
-            "course": "IS103",
-            "section": "S1",
-            "day": "4",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Ivy KHOO",
-            "venue": "Seminar Rm 2-9",
-            "size": "10"
-        },
-        {
-            "course": "IS103",
-            "section": "S2",
-            "day": "5",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Jason KHOO",
-            "venue": "Seminar Rm 2-10",
-            "size": "10"
-        },
-        {
-            "course": "IS103",
-            "section": "S3",
-            "day": "1",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Kat KHOO",
-            "venue": "Seminar Rm 2-11",
-            "size": "10"
-        },
-        {
-            "course": "IS104",
-            "section": "S1",
-            "day": "2",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Linn KHOO",
-            "venue": "Seminar Rm 2-12",
-            "size": "10"
-        },
-        {
-            "course": "IS104",
-            "section": "S2",
-            "day": "3",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Michael KHOO",
-            "venue": "Seminar Rm 2-13",
-            "size": "10"
-        },
-        {
-            "course": "IS105",
-            "section": "S1",
-            "day": "4",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Nathaniel KHOO",
-            "venue": "Seminar Rm 2-14",
-            "size": "10"
-        },
-        {
-            "course": "IS105",
-            "section": "S2",
-            "day": "5",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Oreilly KHOO",
-            "venue": "Seminar Rm 2-15",
-            "size": "10"
-        },
-        {
-            "course": "IS106",
-            "section": "S1",
-            "day": "1",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Peter KHOO",
-            "venue": "Seminar Rm 2-16",
-            "size": "10"
-        },
-        {
-            "course": "IS106",
-            "section": "S2",
-            "day": "2",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Queen KHOO",
-            "venue": "Seminar Rm 2-17",
-            "size": "10"
-        },
-        {
-            "course": "IS107",
-            "section": "S1",
-            "day": "3",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Ray KHOO",
-            "venue": "Seminar Rm 2-18",
-            "size": "10"
-        },
-        {
-            "course": "IS107",
-            "section": "S2",
-            "day": "4",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Simon KHOO",
-            "venue": "Seminar Rm 2-19",
-            "size": "10"
-        },
-        {
-            "course": "IS108",
-            "section": "S1",
-            "day": "5",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Tim KHOO",
-            "venue": "Seminar Rm 2-20",
-            "size": "10"
-        },
-        {
-            "course": "IS109",
-            "section": "S1",
-            "day": "2",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Vincent KHOO",
-            "venue": "Seminar Rm 2-22",
-            "size": "10"
-        },
-        {
-            "course": "IS109",
-            "section": "S2",
-            "day": "3",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Winnie KHOO",
-            "venue": "Seminar Rm 2-23",
-            "size": "10"
-        },
-        {
-            "course": "IS200",
-            "section": "S1",
-            "day": "4",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Xtra KHOO",
-            "venue": "Seminar Rm 2-24",
-            "size": "10"
-        },
-        {
-            "course": "IS201",
-            "section": "S1",
-            "day": "5",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Yale KHOO",
-            "venue": "Seminar Rm 2-25",
-            "size": "10"
-        },
-        {
-            "course": "IS202",
-            "section": "S1",
-            "day": "1",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Zen KHOO",
-            "venue": "Seminar Rm 2-26",
-            "size": "10"
-        },
-        {
-            "course": "IS203",
-            "section": "S1",
-            "day": "2",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Anderson KHOO",
-            "venue": "Seminar Rm 2-27",
-            "size": "10"
-        },
-        {
-            "course": "IS204",
-            "section": "S1",
-            "day": "3",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Bing KHOO",
-            "venue": "Seminar Rm 2-28",
-            "size": "10"
-        },
-        {
-            "course": "IS205",
-            "section": "S1",
-            "day": "4",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Carlo KHOO",
-            "venue": "Seminar Rm 2-29",
-            "size": "10"
-        },
-        {
-            "course": "IS206",
-            "section": "S1",
-            "day": "5",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Dickson KHOO",
-            "venue": "Seminar Rm 2-30",
-            "size": "10"
-        },
-        {
-            "course": "IS207",
-            "section": "S1",
-            "day": "1",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Edmund KHOO",
-            "venue": "Seminar Rm 2-31",
-            "size": "10"
-        },
-        {
-            "course": "IS208",
-            "section": "S1",
-            "day": "2",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Febrice KHOO",
-            "venue": "Seminar Rm 2-32",
-            "size": "10"
-        },
-        {
-            "course": "MGMT001",
-            "section": "S1",
-            "day": "3",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Gavin KHOO",
-            "venue": "Seminar Rm 2-33",
-            "size": "10"
-        },
-        {
-            "course": "MGMT002",
-            "section": "S1",
-            "day": "3",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Bob KHOO",
-            "venue": "Seminar Rm 2-37",
-            "size": "10"
-        }
-    ],
-    "students": [
-        {
-            "userid": "amy.ng.2009",
-            "password": "qwerty128",
-            "name": "Amy NG",
-            "school": "SIS",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "ben.ng.2009",
-            "password": "qwerty129",
-            "name": "Ben NG",
-            "school": "SIS",
-            "edollar": "189.00"
-        },
-        {
-            "userid": "calvin.ng.2009",
-            "password": "qwerty130",
-            "name": "Calvin NG",
-            "school": "SIS",
-            "edollar": "188.00"
-        },
-        {
-            "userid": "dawn.ng.2009",
-            "password": "qwerty131",
-            "name": "Dawn NG",
-            "school": "SIS",
-            "edollar": "187.00"
-        },
-        {
-            "userid": "eddy.ng.2009",
-            "password": "qwerty132",
-            "name": "Eddy NG",
-            "school": "SIS",
-            "edollar": "186.00"
-        },
-        {
-            "userid": "fred.ng.2009",
-            "password": "qwerty133",
-            "name": "Fred NG",
-            "school": "SIS",
-            "edollar": "185.00"
-        },
-        {
-            "userid": "gary.ng.2009",
-            "password": "qwerty134",
-            "name": "Gary NG",
-            "school": "SIS",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "harry.ng.2009",
-            "password": "qwerty135",
-            "name": "Harry NG",
-            "school": "SIS",
-            "edollar": "183.00"
-        },
-        {
-            "userid": "ian.ng.2009",
-            "password": "qwerty136",
-            "name": "Ian NG",
-            "school": "SIS",
-            "edollar": "182.00"
-        },
-        {
-            "userid": "jerry.ng.2009",
-            "password": "qwerty137",
-            "name": "Jerry NG",
-            "school": "SIS",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "kelly.ng.2009",
-            "password": "qwerty138",
-            "name": "Kelly NG",
-            "school": "SIS",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "larry.ng.2009",
-            "password": "qwerty139",
-            "name": "Larry NG",
-            "school": "SIS",
-            "edollar": "181.00"
-        },
-        {
-            "userid": "maggie.ng.2009",
-            "password": "qwerty140",
-            "name": "Maggie NG",
-            "school": "SIS",
-            "edollar": "180.00"
-        },
-        {
-            "userid": "neilson.ng.2009",
-            "password": "qwerty141",
-            "name": "Neilson NG",
-            "school": "SIS",
-            "edollar": "179.00"
-        },
-        {
-            "userid": "olivia.ng.2009",
-            "password": "qwerty142",
-            "name": "Olivia NG",
-            "school": "SIS",
-            "edollar": "178.00"
-        },
-        {
-            "userid": "parker.ng.2009",
-            "password": "qwerty143",
-            "name": "Parker NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "quiten.ng.2009",
-            "password": "qwerty144",
-            "name": "Quiten NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "ricky.ng.2009",
-            "password": "qwerty145",
-            "name": "Ricky NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "steven.ng.2009",
-            "password": "qwerty146",
-            "name": "Steven NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "timothy.ng.2009",
-            "password": "qwerty147",
-            "name": "Timothy NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "ursala.ng.2009",
-            "password": "qwerty148",
-            "name": "Ursala NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "valarie.ng.2009",
-            "password": "qwerty149",
-            "name": "Valarie NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "winston.ng.2009",
-            "password": "qwerty150",
-            "name": "Winston NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "xavier.ng.2009",
-            "password": "qwerty151",
-            "name": "Xavier NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "yasir.ng.2009",
-            "password": "qwerty152",
-            "name": "Yasir NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "zac.ng.2009",
-            "password": "qwerty153",
-            "name": "Zac NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        }
-    ],
-    "prerequisite": [
-        {
-            "course": "IS101",
-            "prerequisite": "IS100"
-        },
-        {
-            "course": "IS103",
-            "prerequisite": "IS102"
-        },
-        {
-            "course": "IS104",
-            "prerequisite": "IS103"
-        },
-        {
-            "course": "IS109",
-            "prerequisite": "IS102"
-        },
-        {
-            "course": "IS203",
-            "prerequisite": "IS103"
-        },
-        {
-            "course": "IS203",
-            "prerequisite": "IS106"
-        },
-        {
-            "course": "IS204",
-            "prerequisite": "IS106"
-        },
-        {
-            "course": "IS209",
-            "prerequisite": "IS106"
-        }
-    ],
-    "bid": [
-        {
-            "userid": "olivia.ng.2009",
-            "amount": "22.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "neilson.ng.2009",
-            "amount": "21.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "maggie.ng.2009",
-            "amount": "20.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "larry.ng.2009",
-            "amount": "19.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "ian.ng.2009",
-            "amount": "18.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "harry.ng.2009",
-            "amount": "17.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "fred.ng.2009",
-            "amount": "15.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "eddy.ng.2009",
-            "amount": "14.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "dawn.ng.2009",
-            "amount": "13.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "calvin.ng.2009",
-            "amount": "12.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "ben.ng.2009",
-            "amount": "11.00",
-            "course": "IS100",
-            "section": "S1"
-        }
-    ],
-    "completed-course": [
-        {
-            "userid": "amy.ng.2009",
-            "course": "IS100"
-        },
-        {
-            "userid": "gary.ng.2009",
-            "course": "IS100"
-        },
-        {
-            "userid": "ben.ng.2009",
-            "course": "IS102"
-        },
-        {
-            "userid": "ben.ng.2009",
-            "course": "IS103"
-        }
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "error",
-    "message": [
-        "invalid userid"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>Authentication</t>
-  </si>
-  <si>
-    <t>Stop round</t>
-  </si>
-  <si>
-    <t>Start round</t>
-  </si>
-  <si>
-    <t>Dump</t>
-  </si>
-  <si>
-    <t>{
-    "status": "error",
-    "message": [
-        "invalid amount"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "error",
-    "message": [
-        "invalid course"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>Update bid - succesful case</t>
-  </si>
-  <si>
-    <t>Update bid - enter invalid user</t>
-  </si>
-  <si>
-    <t>Update bid - enter invalid amount</t>
-  </si>
-  <si>
-    <t>Update bid - enter invalid course</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2735,16 +1750,16 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
+    <row r="1" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2770,7 +1785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2780,7 +1795,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="60">
+    <row r="3" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2806,7 +1821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="75">
+    <row r="4" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2832,7 +1847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60">
+    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2858,7 +1873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60">
+    <row r="6" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2884,7 +1899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60">
+    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2910,7 +1925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45">
+    <row r="8" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2936,7 +1951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45">
+    <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2962,7 +1977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60">
+    <row r="10" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2988,7 +2003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3014,7 +2029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3040,7 +2055,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3066,7 +2081,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="120">
+    <row r="14" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -3092,7 +2107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="120">
+    <row r="15" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -3118,7 +2133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -3144,7 +2159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45">
+    <row r="17" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -3170,7 +2185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -3196,7 +2211,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="75">
+    <row r="19" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -3222,7 +2237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45">
+    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -3248,7 +2263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="120">
+    <row r="21" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -3274,7 +2289,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45">
+    <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -3300,7 +2315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="45">
+    <row r="23" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -3326,7 +2341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45">
+    <row r="24" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -3352,7 +2367,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45">
+    <row r="25" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -3378,7 +2393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45">
+    <row r="26" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -3404,7 +2419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="60">
+    <row r="27" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -3430,7 +2445,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45">
+    <row r="28" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -3456,7 +2471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="105">
+    <row r="29" spans="1:8" ht="98" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -3482,7 +2497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="409.6">
+    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -3508,7 +2523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="225">
+    <row r="31" spans="1:8" ht="224" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -3534,7 +2549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="45">
+    <row r="32" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -3560,7 +2575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45">
+    <row r="33" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -3586,7 +2601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="45">
+    <row r="34" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -3612,7 +2627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="45">
+    <row r="35" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -3638,7 +2653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="45">
+    <row r="36" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -3664,7 +2679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="45">
+    <row r="37" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -3690,7 +2705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="60">
+    <row r="38" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -3716,7 +2731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="45">
+    <row r="39" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -3742,7 +2757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="105">
+    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -3768,7 +2783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="105">
+    <row r="41" spans="1:8" ht="98" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -3794,7 +2809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="45">
+    <row r="42" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -3820,7 +2835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="45">
+    <row r="43" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -3846,7 +2861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="165">
+    <row r="44" spans="1:8" ht="154" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -3872,7 +2887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="60">
+    <row r="45" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -3898,7 +2913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="60">
+    <row r="46" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -3924,7 +2939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="45">
+    <row r="47" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -3950,7 +2965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="60">
+    <row r="48" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -3976,7 +2991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="60">
+    <row r="49" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -4002,7 +3017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45">
+    <row r="50" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -4028,7 +3043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="45">
+    <row r="51" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -4054,7 +3069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="45">
+    <row r="52" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -4080,7 +3095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="45">
+    <row r="53" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -4106,7 +3121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="45">
+    <row r="54" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -4132,7 +3147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="60">
+    <row r="55" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -4158,7 +3173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="60">
+    <row r="56" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -4206,20 +3221,20 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.5" customWidth="1"/>
-    <col min="4" max="4" width="78.5" customWidth="1"/>
-    <col min="5" max="5" width="78.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="78.453125" customWidth="1"/>
+    <col min="5" max="5" width="78.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4239,7 +3254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" customHeight="1">
+    <row r="2" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -4247,7 +3262,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="105">
+    <row r="3" spans="1:6" ht="98" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -4267,7 +3282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60">
+    <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -4287,7 +3302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60">
+    <row r="5" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -4307,7 +3322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60">
+    <row r="6" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -4348,17 +3363,17 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="33.6328125" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4378,7 +3393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1">
+    <row r="2" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -4386,7 +3401,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="180">
+    <row r="3" spans="1:6" ht="168" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -4406,7 +3421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.6">
+    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -4447,16 +3462,16 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4482,7 +3497,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -4492,7 +3507,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1">
+    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4518,7 +3533,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1">
+    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4544,7 +3559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4570,7 +3585,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45">
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4596,7 +3611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45">
+    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4622,7 +3637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45">
+    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4648,7 +3663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60">
+    <row r="9" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4674,7 +3689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="75">
+    <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4700,7 +3715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="75">
+    <row r="11" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4726,7 +3741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="75">
+    <row r="12" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4752,7 +3767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4778,7 +3793,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45">
+    <row r="14" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4804,7 +3819,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30">
+    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4830,7 +3845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="75">
+    <row r="16" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4856,7 +3871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="75">
+    <row r="17" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4882,7 +3897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4908,7 +3923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45">
+    <row r="19" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4934,7 +3949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60">
+    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4960,7 +3975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45">
+    <row r="21" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4986,7 +4001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45">
+    <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5012,7 +4027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="75">
+    <row r="23" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -5038,7 +4053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30">
+    <row r="24" spans="1:8" ht="28" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -5064,7 +4079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14">
+    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5074,7 +4089,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14">
+    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5084,7 +4099,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14">
+    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5094,7 +4109,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14">
+    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5104,7 +4119,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14">
+    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5114,7 +4129,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14">
+    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5124,7 +4139,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14">
+    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5134,7 +4149,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14">
+    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5144,7 +4159,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14">
+    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5154,7 +4169,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14">
+    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5164,7 +4179,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14">
+    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5174,7 +4189,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14">
+    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5184,7 +4199,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14">
+    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5194,7 +4209,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14">
+    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5204,7 +4219,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14">
+    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -5214,7 +4229,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14">
+    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -5224,7 +4239,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14">
+    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5234,7 +4249,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14">
+    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5244,7 +4259,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14">
+    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -5254,7 +4269,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14">
+    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -5264,7 +4279,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14">
+    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -5274,7 +4289,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14">
+    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -5284,7 +4299,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14">
+    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -5294,7 +4309,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14">
+    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -5304,7 +4319,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14">
+    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -5314,7 +4329,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14">
+    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -5324,7 +4339,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14">
+    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5334,7 +4349,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14">
+    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5344,7 +4359,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14">
+    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -5354,7 +4369,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14">
+    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -5364,7 +4379,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14">
+    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -5374,7 +4389,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14">
+    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
@@ -5400,395 +4415,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED20DAA-AFB2-5240-A261-8BB8E5918D09}">
-  <dimension ref="A1:F22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
-  <cols>
-    <col min="3" max="3" width="30.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" ht="150">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="64" customHeight="1">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="77" customHeight="1">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="90">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="409.6">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="52" customHeight="1">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="90">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="90">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="90">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="14">
-      <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="14">
-      <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="14">
-      <c r="A20" s="2">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="14">
-      <c r="A21" s="2">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="14">
-      <c r="A22" s="2">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA8D5A-5628-41F0-8C3D-F219DADB62EC}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5814,7 +4457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -5824,7 +4467,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1">
+    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5850,7 +4493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1">
+    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5876,7 +4519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45">
+    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5902,7 +4545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="75">
+    <row r="6" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5928,7 +4571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75">
+    <row r="7" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5954,7 +4597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="90">
+    <row r="8" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5980,7 +4623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60">
+    <row r="9" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6006,7 +4649,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45">
+    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6020,19 +4663,19 @@
         <v>318</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6043,48 +4686,32 @@
         <v>317</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>322</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="14">
+    <row r="12" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -6094,7 +4721,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="14">
+    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -6104,7 +4731,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14">
+    <row r="15" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -6114,7 +4741,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="14">
+    <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
@@ -6124,7 +4751,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="14">
+    <row r="17" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
@@ -6134,7 +4761,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="14">
+    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6144,7 +4771,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="14">
+    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6154,7 +4781,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="14">
+    <row r="20" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6164,7 +4791,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="14">
+    <row r="21" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6174,7 +4801,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="14">
+    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6184,7 +4811,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="14">
+    <row r="23" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6194,7 +4821,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="14">
+    <row r="24" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6204,7 +4831,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="14">
+    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6214,7 +4841,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14">
+    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6224,7 +4851,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14">
+    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6234,7 +4861,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14">
+    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6244,7 +4871,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14">
+    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6254,7 +4881,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14">
+    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6264,7 +4891,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14">
+    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6274,7 +4901,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14">
+    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6284,7 +4911,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14">
+    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6294,7 +4921,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14">
+    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6304,7 +4931,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14">
+    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6314,7 +4941,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14">
+    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -6324,7 +4951,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14">
+    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6334,7 +4961,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14">
+    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6344,7 +4971,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14">
+    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -6354,7 +4981,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14">
+    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -6364,7 +4991,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14">
+    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -6374,7 +5001,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14">
+    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -6384,7 +5011,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14">
+    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -6394,7 +5021,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14">
+    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -6404,7 +5031,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14">
+    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -6414,7 +5041,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14">
+    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -6424,7 +5051,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14">
+    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -6434,7 +5061,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14">
+    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -6444,7 +5071,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14">
+    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -6454,7 +5081,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14">
+    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -6464,7 +5091,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14">
+    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -6474,7 +5101,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14">
+    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -6484,7 +5111,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14">
+    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6494,7 +5121,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14">
+    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -6504,7 +5131,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14">
+    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -6514,7 +5141,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14">
+    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>

</xml_diff>

<commit_message>
Revert "Revert "JSON testcases updated in excel file""
This reverts commit 01dddabb0b10fdea3b2d4d8312d41cedc04b8984.
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rou Hui\Documents\GitHub\project-g3t4\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amey/Documents/GitHub/project-g3t4/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39E3E23-BA92-47E7-962C-53E42B62672D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3213DF3F-6A19-2545-A9E1-8E0E3EF25A9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1 – Manual – Login Bo" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 1 - JSON - Login" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 1 – JSON – Authentica" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration 2 - Manual - Round 1" sheetId="4" r:id="rId4"/>
-    <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId5"/>
+    <sheet name="Iteration 2 -- JSON" sheetId="6" r:id="rId5"/>
+    <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="351">
   <si>
     <t>S/N</t>
   </si>
@@ -1341,26 +1342,1010 @@
     <t>student bids for section that has 0 vancancies with the minimum bid</t>
   </si>
   <si>
-    <t xml:space="preserve">ben.ong bids e$12 for IS100 </t>
-  </si>
-  <si>
     <t>"Pending, fail"</t>
   </si>
   <si>
     <t>student bids for section that has vacancies with the minimum bid</t>
   </si>
   <si>
-    <t>ben.ong bids for e$14.01 for IS100</t>
-  </si>
-  <si>
     <t>"Pending, successful"</t>
+  </si>
+  <si>
+    <t>ben.ng bids for e$14.01 for IS100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ben.ng bids e$12 for IS100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 students bid the same amount for one vacancy </t>
+  </si>
+  <si>
+    <t>ben.ng and za.ng bid e$10 for is100</t>
+  </si>
+  <si>
+    <t>both unsucessful</t>
+  </si>
+  <si>
+    <t>error thrown</t>
+  </si>
+  <si>
+    <t>username=calvin.ng.2009</t>
+  </si>
+  <si>
+    <t>username=calvin.ng.2009
+password=qwerty130</t>
+  </si>
+  <si>
+    <t>username=calvin.ng.2009
+password=wrongpasswordhaha</t>
+  </si>
+  <si>
+    <t>EMPTY</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS102","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "ada.goh.2012","amount": 11.0,"course": "IS100","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","amount": 9.0,"course": "IS100","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS110","section": "S1"}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "round not started"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "round": "1"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "courses": [
+        {
+            "course": "ECON001",
+            "school": "SOE",
+            "title": "Microeconomics",
+            "description": "Microeconomics is about economics in smaller scale (e.g. firm-scale)",
+            "examdate": "20131101",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "ECON002",
+            "school": "SOE",
+            "title": "Macroeconomics",
+            "description": "You don't learn about excel macros here.",
+            "examdate": "20131101",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS100",
+            "school": "SIS",
+            "title": "Calculus ",
+            "description": "The basic objective of Calculus is to relate small-scale (differential) quantities to large-scale (integrated) quantities. This is accomplished by means of the Fundamental Theorem of Calculus. Students should demonstrate an understanding of the integral as a cumulative sum, of the derivative as a rate of change, and of the inverse relationship between integration and differentiation.",
+            "examdate": "20131119",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS101",
+            "school": "SIS",
+            "title": "Advanced Calculus",
+            "description": "This is a second course on calculus.\u00a0It is more advanced definitely.",
+            "examdate": "20131118",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS102",
+            "school": "SIS",
+            "title": "Java programming",
+            "description": "This course teaches you on Java programming. I love Java definitely.",
+            "examdate": "20131117",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS103",
+            "school": "SIS",
+            "title": "Web Programming",
+            "description": "JSP, Servlets using Tomcat",
+            "examdate": "20131116",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS104",
+            "school": "SIS",
+            "title": "Advanced Programming",
+            "description": "How to write code that nobody can understand",
+            "examdate": "20131115",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS105",
+            "school": "SIS",
+            "title": "Data Structures",
+            "description": "Data structure is a particular way of storing and organizing data in a computer so that it can be used efficiently. Arrays, Lists, Stacks and Trees will be covered.",
+            "examdate": "20131114",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS106",
+            "school": "SIS",
+            "title": "Database Modeling &amp; Design",
+            "description": "Data modeling in software engineering is the process of creating a data model by applying formal data model descriptions using data modeling techniques. ",
+            "examdate": "20131113",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS107",
+            "school": "SIS",
+            "title": "IT Outsourcing",
+            "description": "This course teaches you on how to outsource your programming projects to others.",
+            "examdate": "20131112",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS108",
+            "school": "SIS",
+            "title": "Organization Behaviour",
+            "description": "Organizational Behavior (OB) is the study and application of knowledge about how people, individuals, and groups act in organizations. ",
+            "examdate": "20131111",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS109",
+            "school": "SIS",
+            "title": "Cloud Computing",
+            "description": "Cloud computing is Internet-based computing, whereby shared resources, software and information are provided to computers and other devices on-demand, like the electricity grid.",
+            "examdate": "20131110",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS200",
+            "school": "SIS",
+            "title": "Final Touch",
+            "description": "Learn how eat, dress and talk.",
+            "examdate": "20131109",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS201",
+            "school": "SIS",
+            "title": "Fun with Shell Programming",
+            "description": "Shell scripts are a fundamental part of the UNIX and Linux programming environment.",
+            "examdate": "20131108",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS202",
+            "school": "SIS",
+            "title": "Enterprise integration",
+            "description": "Enterprise integration is a technical field of Enterprise Architecture, which focused on the study of things like system interconnection, electronic data interchange, product data exchange and distributed computing environments, and it's possible other solutions.[1",
+            "examdate": "20131107",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS203",
+            "school": "SIS",
+            "title": "Software Engineering",
+            "description": "The Sleepless Era.",
+            "examdate": "20131106",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS204",
+            "school": "SIS",
+            "title": "Database System Administration",
+            "description": "Database administration is a complex, often thankless chore.",
+            "examdate": "20131105",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS205",
+            "school": "SIS",
+            "title": "All Talk, No Action",
+            "description": "The easiest course of all. We will sit around and talk.",
+            "examdate": "20131104",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS206",
+            "school": "SIS",
+            "title": "Operation Research",
+            "description": "Operations research, also known as operational research, is an interdisciplinary branch of applied mathematics and formal science that uses advanced analytical methods such as mathematical modeling, statistical analysis, and mathematical optimization to arrive at optimal or near-optimal solutions to complex decision-making problems.",
+            "examdate": "20131103",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "IS207",
+            "school": "SIS",
+            "title": "GUI Bloopers",
+            "description": "Common User Interface Design Don'ts and Dos",
+            "examdate": "20131103",
+            "examstart": "15:30:00",
+            "examend": "18:45:00"
+        },
+        {
+            "course": "IS208",
+            "school": "SIS",
+            "title": "Artifical Intelligence",
+            "description": "The science and engineering of making intelligent machine",
+            "examdate": "20131103",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "IS209",
+            "school": "SIS",
+            "title": "Information Storage and Management",
+            "description": "Information storage and management (ISM) - once a relatively straightforward operation -has developed into a highly sophisticated pillar of information technology, requiring proven technical expertise.",
+            "examdate": "20131102",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        },
+        {
+            "course": "MGMT001",
+            "school": "SOB",
+            "title": "Business,Government, and Society",
+            "description": "learn the interrelation amongst the three",
+            "examdate": "20131102",
+            "examstart": "08:30:00",
+            "examend": "11:45:00"
+        },
+        {
+            "course": "MGMT002",
+            "school": "SOB",
+            "title": "Technology and World Change",
+            "description": "As technology changes, so does the world",
+            "examdate": "20131101",
+            "examstart": "12:00:00",
+            "examend": "15:15:00"
+        }
+    ],
+    "section": [
+        {
+            "course": "ECON001",
+            "section": "S1",
+            "day": "4",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "John KHOO",
+            "venue": "Seminar Rm 2-34",
+            "size": "10"
+        },
+        {
+            "course": "ECON002",
+            "section": "S1",
+            "day": "5",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Andy KHOO",
+            "venue": "Seminar Rm 2-35",
+            "size": "10"
+        },
+        {
+            "course": "IS100",
+            "section": "S1",
+            "day": "1",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Albert KHOO",
+            "venue": "Seminar Rm 2-1",
+            "size": "10"
+        },
+        {
+            "course": "IS100",
+            "section": "S2",
+            "day": "2",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Billy KHOO",
+            "venue": "Seminar Rm 2-2",
+            "size": "10"
+        },
+        {
+            "course": "IS101",
+            "section": "S1",
+            "day": "3",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Cheri KHOO",
+            "venue": "Seminar Rm 2-3",
+            "size": "10"
+        },
+        {
+            "course": "IS101",
+            "section": "S2",
+            "day": "4",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Daniel KHOO",
+            "venue": "Seminar Rm 2-4",
+            "size": "10"
+        },
+        {
+            "course": "IS101",
+            "section": "S3",
+            "day": "5",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Ernest KHOO",
+            "venue": "Seminar Rm 2-5",
+            "size": "10"
+        },
+        {
+            "course": "IS102",
+            "section": "S1",
+            "day": "1",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Felicia KHOO",
+            "venue": "Seminar Rm 2-6",
+            "size": "10"
+        },
+        {
+            "course": "IS102",
+            "section": "S2",
+            "day": "2",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Gerald KHOO",
+            "venue": "Seminar Rm 2-7",
+            "size": "10"
+        },
+        {
+            "course": "IS102",
+            "section": "S3",
+            "day": "3",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Henry KHOO",
+            "venue": "Seminar Rm 2-8",
+            "size": "10"
+        },
+        {
+            "course": "IS103",
+            "section": "S1",
+            "day": "4",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Ivy KHOO",
+            "venue": "Seminar Rm 2-9",
+            "size": "10"
+        },
+        {
+            "course": "IS103",
+            "section": "S2",
+            "day": "5",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Jason KHOO",
+            "venue": "Seminar Rm 2-10",
+            "size": "10"
+        },
+        {
+            "course": "IS103",
+            "section": "S3",
+            "day": "1",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Kat KHOO",
+            "venue": "Seminar Rm 2-11",
+            "size": "10"
+        },
+        {
+            "course": "IS104",
+            "section": "S1",
+            "day": "2",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Linn KHOO",
+            "venue": "Seminar Rm 2-12",
+            "size": "10"
+        },
+        {
+            "course": "IS104",
+            "section": "S2",
+            "day": "3",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Michael KHOO",
+            "venue": "Seminar Rm 2-13",
+            "size": "10"
+        },
+        {
+            "course": "IS105",
+            "section": "S1",
+            "day": "4",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Nathaniel KHOO",
+            "venue": "Seminar Rm 2-14",
+            "size": "10"
+        },
+        {
+            "course": "IS105",
+            "section": "S2",
+            "day": "5",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Oreilly KHOO",
+            "venue": "Seminar Rm 2-15",
+            "size": "10"
+        },
+        {
+            "course": "IS106",
+            "section": "S1",
+            "day": "1",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Peter KHOO",
+            "venue": "Seminar Rm 2-16",
+            "size": "10"
+        },
+        {
+            "course": "IS106",
+            "section": "S2",
+            "day": "2",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Queen KHOO",
+            "venue": "Seminar Rm 2-17",
+            "size": "10"
+        },
+        {
+            "course": "IS107",
+            "section": "S1",
+            "day": "3",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Ray KHOO",
+            "venue": "Seminar Rm 2-18",
+            "size": "10"
+        },
+        {
+            "course": "IS107",
+            "section": "S2",
+            "day": "4",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Simon KHOO",
+            "venue": "Seminar Rm 2-19",
+            "size": "10"
+        },
+        {
+            "course": "IS108",
+            "section": "S1",
+            "day": "5",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Tim KHOO",
+            "venue": "Seminar Rm 2-20",
+            "size": "10"
+        },
+        {
+            "course": "IS109",
+            "section": "S1",
+            "day": "2",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Vincent KHOO",
+            "venue": "Seminar Rm 2-22",
+            "size": "10"
+        },
+        {
+            "course": "IS109",
+            "section": "S2",
+            "day": "3",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Winnie KHOO",
+            "venue": "Seminar Rm 2-23",
+            "size": "10"
+        },
+        {
+            "course": "IS200",
+            "section": "S1",
+            "day": "4",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Xtra KHOO",
+            "venue": "Seminar Rm 2-24",
+            "size": "10"
+        },
+        {
+            "course": "IS201",
+            "section": "S1",
+            "day": "5",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Yale KHOO",
+            "venue": "Seminar Rm 2-25",
+            "size": "10"
+        },
+        {
+            "course": "IS202",
+            "section": "S1",
+            "day": "1",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Zen KHOO",
+            "venue": "Seminar Rm 2-26",
+            "size": "10"
+        },
+        {
+            "course": "IS203",
+            "section": "S1",
+            "day": "2",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Anderson KHOO",
+            "venue": "Seminar Rm 2-27",
+            "size": "10"
+        },
+        {
+            "course": "IS204",
+            "section": "S1",
+            "day": "3",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Bing KHOO",
+            "venue": "Seminar Rm 2-28",
+            "size": "10"
+        },
+        {
+            "course": "IS205",
+            "section": "S1",
+            "day": "4",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Carlo KHOO",
+            "venue": "Seminar Rm 2-29",
+            "size": "10"
+        },
+        {
+            "course": "IS206",
+            "section": "S1",
+            "day": "5",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Dickson KHOO",
+            "venue": "Seminar Rm 2-30",
+            "size": "10"
+        },
+        {
+            "course": "IS207",
+            "section": "S1",
+            "day": "1",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Edmund KHOO",
+            "venue": "Seminar Rm 2-31",
+            "size": "10"
+        },
+        {
+            "course": "IS208",
+            "section": "S1",
+            "day": "2",
+            "start": "12:00:00",
+            "end": "15:15:00",
+            "instructor": "Febrice KHOO",
+            "venue": "Seminar Rm 2-32",
+            "size": "10"
+        },
+        {
+            "course": "MGMT001",
+            "section": "S1",
+            "day": "3",
+            "start": "08:30:00",
+            "end": "11:45:00",
+            "instructor": "Gavin KHOO",
+            "venue": "Seminar Rm 2-33",
+            "size": "10"
+        },
+        {
+            "course": "MGMT002",
+            "section": "S1",
+            "day": "3",
+            "start": "15:30:00",
+            "end": "18:45:00",
+            "instructor": "Bob KHOO",
+            "venue": "Seminar Rm 2-37",
+            "size": "10"
+        }
+    ],
+    "students": [
+        {
+            "userid": "amy.ng.2009",
+            "password": "qwerty128",
+            "name": "Amy NG",
+            "school": "SIS",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "password": "qwerty129",
+            "name": "Ben NG",
+            "school": "SIS",
+            "edollar": "189.00"
+        },
+        {
+            "userid": "calvin.ng.2009",
+            "password": "qwerty130",
+            "name": "Calvin NG",
+            "school": "SIS",
+            "edollar": "188.00"
+        },
+        {
+            "userid": "dawn.ng.2009",
+            "password": "qwerty131",
+            "name": "Dawn NG",
+            "school": "SIS",
+            "edollar": "187.00"
+        },
+        {
+            "userid": "eddy.ng.2009",
+            "password": "qwerty132",
+            "name": "Eddy NG",
+            "school": "SIS",
+            "edollar": "186.00"
+        },
+        {
+            "userid": "fred.ng.2009",
+            "password": "qwerty133",
+            "name": "Fred NG",
+            "school": "SIS",
+            "edollar": "185.00"
+        },
+        {
+            "userid": "gary.ng.2009",
+            "password": "qwerty134",
+            "name": "Gary NG",
+            "school": "SIS",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "harry.ng.2009",
+            "password": "qwerty135",
+            "name": "Harry NG",
+            "school": "SIS",
+            "edollar": "183.00"
+        },
+        {
+            "userid": "ian.ng.2009",
+            "password": "qwerty136",
+            "name": "Ian NG",
+            "school": "SIS",
+            "edollar": "182.00"
+        },
+        {
+            "userid": "jerry.ng.2009",
+            "password": "qwerty137",
+            "name": "Jerry NG",
+            "school": "SIS",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "kelly.ng.2009",
+            "password": "qwerty138",
+            "name": "Kelly NG",
+            "school": "SIS",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "larry.ng.2009",
+            "password": "qwerty139",
+            "name": "Larry NG",
+            "school": "SIS",
+            "edollar": "181.00"
+        },
+        {
+            "userid": "maggie.ng.2009",
+            "password": "qwerty140",
+            "name": "Maggie NG",
+            "school": "SIS",
+            "edollar": "180.00"
+        },
+        {
+            "userid": "neilson.ng.2009",
+            "password": "qwerty141",
+            "name": "Neilson NG",
+            "school": "SIS",
+            "edollar": "179.00"
+        },
+        {
+            "userid": "olivia.ng.2009",
+            "password": "qwerty142",
+            "name": "Olivia NG",
+            "school": "SIS",
+            "edollar": "178.00"
+        },
+        {
+            "userid": "parker.ng.2009",
+            "password": "qwerty143",
+            "name": "Parker NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "quiten.ng.2009",
+            "password": "qwerty144",
+            "name": "Quiten NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "ricky.ng.2009",
+            "password": "qwerty145",
+            "name": "Ricky NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "steven.ng.2009",
+            "password": "qwerty146",
+            "name": "Steven NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "timothy.ng.2009",
+            "password": "qwerty147",
+            "name": "Timothy NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "ursala.ng.2009",
+            "password": "qwerty148",
+            "name": "Ursala NG",
+            "school": "SOE",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "valarie.ng.2009",
+            "password": "qwerty149",
+            "name": "Valarie NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "winston.ng.2009",
+            "password": "qwerty150",
+            "name": "Winston NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "xavier.ng.2009",
+            "password": "qwerty151",
+            "name": "Xavier NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "yasir.ng.2009",
+            "password": "qwerty152",
+            "name": "Yasir NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        },
+        {
+            "userid": "zac.ng.2009",
+            "password": "qwerty153",
+            "name": "Zac NG",
+            "school": "SOB",
+            "edollar": "200.00"
+        }
+    ],
+    "prerequisite": [
+        {
+            "course": "IS101",
+            "prerequisite": "IS100"
+        },
+        {
+            "course": "IS103",
+            "prerequisite": "IS102"
+        },
+        {
+            "course": "IS104",
+            "prerequisite": "IS103"
+        },
+        {
+            "course": "IS109",
+            "prerequisite": "IS102"
+        },
+        {
+            "course": "IS203",
+            "prerequisite": "IS103"
+        },
+        {
+            "course": "IS203",
+            "prerequisite": "IS106"
+        },
+        {
+            "course": "IS204",
+            "prerequisite": "IS106"
+        },
+        {
+            "course": "IS209",
+            "prerequisite": "IS106"
+        }
+    ],
+    "bid": [
+        {
+            "userid": "olivia.ng.2009",
+            "amount": "22.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "neilson.ng.2009",
+            "amount": "21.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "maggie.ng.2009",
+            "amount": "20.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "larry.ng.2009",
+            "amount": "19.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "ian.ng.2009",
+            "amount": "18.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "harry.ng.2009",
+            "amount": "17.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "fred.ng.2009",
+            "amount": "15.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "eddy.ng.2009",
+            "amount": "14.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "dawn.ng.2009",
+            "amount": "13.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "calvin.ng.2009",
+            "amount": "12.00",
+            "course": "IS100",
+            "section": "S1"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "amount": "11.00",
+            "course": "IS100",
+            "section": "S1"
+        }
+    ],
+    "completed-course": [
+        {
+            "userid": "amy.ng.2009",
+            "course": "IS100"
+        },
+        {
+            "userid": "gary.ng.2009",
+            "course": "IS100"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "course": "IS102"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "course": "IS103"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid userid"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Stop round</t>
+  </si>
+  <si>
+    <t>Start round</t>
+  </si>
+  <si>
+    <t>Dump</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid amount"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid course"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Update bid - succesful case</t>
+  </si>
+  <si>
+    <t>Update bid - enter invalid user</t>
+  </si>
+  <si>
+    <t>Update bid - enter invalid amount</t>
+  </si>
+  <si>
+    <t>Update bid - enter invalid course</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1750,16 +2735,16 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +2770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1795,7 +2780,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1821,7 +2806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="75">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1847,7 +2832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1873,7 +2858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="60">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1899,7 +2884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1925,7 +2910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1951,7 +2936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1977,7 +2962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="60">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2003,7 +2988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2029,7 +3014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2055,7 +3040,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2081,7 +3066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="120">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2107,7 +3092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="120">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2133,7 +3118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2159,7 +3144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2185,7 +3170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="45">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2211,7 +3196,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="75">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2237,7 +3222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="45">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2263,7 +3248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="120">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2289,7 +3274,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="45">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2315,7 +3300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="45">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2341,7 +3326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2367,7 +3352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="45">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2393,7 +3378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -2419,7 +3404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="60">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -2445,7 +3430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="45">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -2471,7 +3456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="98" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="105">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -2497,7 +3482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="409.6">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -2523,7 +3508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="224" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="225">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -2549,7 +3534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="45">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -2575,7 +3560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="45">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2601,7 +3586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="45">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -2627,7 +3612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="45">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -2653,7 +3638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="45">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -2679,7 +3664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="45">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -2705,7 +3690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="60">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -2731,7 +3716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="45">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -2757,7 +3742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="105">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -2783,7 +3768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="98" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="105">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -2809,7 +3794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="45">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -2835,7 +3820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="45">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -2861,7 +3846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="154" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="165">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -2887,7 +3872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="60">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -2913,7 +3898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="60">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -2939,7 +3924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="45">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -2965,7 +3950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="60">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -2991,7 +3976,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="60">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -3017,7 +4002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="45">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -3043,7 +4028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="45">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -3069,7 +4054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="45">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -3095,7 +4080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="45">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -3121,7 +4106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="45">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -3147,7 +4132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="60">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -3173,7 +4158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="60">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -3221,20 +4206,20 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView zoomScale="111" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="32.453125" customWidth="1"/>
-    <col min="4" max="4" width="78.453125" customWidth="1"/>
-    <col min="5" max="5" width="78.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="78.5" customWidth="1"/>
+    <col min="5" max="5" width="78.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +4239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="51.75" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -3262,7 +4247,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="98" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="105">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3282,7 +4267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3302,7 +4287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -3322,7 +4307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="60">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -3363,17 +4348,17 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6328125" customWidth="1"/>
-    <col min="5" max="5" width="32.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3393,7 +4378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="48" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -3401,7 +4386,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="168" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="180">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -3421,7 +4406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="409.6">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -3462,16 +4447,16 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
   <cols>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3497,7 +4482,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3507,7 +4492,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="66" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3533,7 +4518,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="63" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3559,7 +4544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3585,7 +4570,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3611,7 +4596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3637,7 +4622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3663,7 +4648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="60">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3689,7 +4674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3715,7 +4700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3741,7 +4726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3767,7 +4752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3793,7 +4778,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3819,7 +4804,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3845,7 +4830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="75">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3871,7 +4856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="75">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3897,7 +4882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="45">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3923,7 +4908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="45">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3949,7 +4934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="60">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3975,7 +4960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="45">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4001,7 +4986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="45">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4027,7 +5012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="75">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4053,7 +5038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -4079,7 +5064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4089,7 +5074,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="14">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4099,7 +5084,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4109,7 +5094,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4119,7 +5104,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4129,7 +5114,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4139,7 +5124,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4149,7 +5134,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4159,7 +5144,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="14">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4169,7 +5154,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="14">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4179,7 +5164,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="14">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4189,7 +5174,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="14">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4199,7 +5184,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="14">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4209,7 +5194,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4219,7 +5204,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="14">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4229,7 +5214,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="14">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4239,7 +5224,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="14">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -4249,7 +5234,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="14">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -4259,7 +5244,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="14">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -4269,7 +5254,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="14">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -4279,7 +5264,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="14">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -4289,7 +5274,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="14">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -4299,7 +5284,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="14">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -4309,7 +5294,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="14">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -4319,7 +5304,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="14">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4329,7 +5314,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="14">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -4339,7 +5324,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="14">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -4349,7 +5334,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="14">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -4359,7 +5344,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="14">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -4369,7 +5354,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="14">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -4379,7 +5364,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="14">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4389,7 +5374,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="14">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
@@ -4415,23 +5400,395 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED20DAA-AFB2-5240-A261-8BB8E5918D09}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <cols>
+    <col min="3" max="3" width="30.1640625" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="48" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="150">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="64" customHeight="1">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="77" customHeight="1">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="409.6">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="52" customHeight="1">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="90">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="14">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="14">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="14">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="14">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA8D5A-5628-41F0-8C3D-F219DADB62EC}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="C7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
   <cols>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4457,7 +5814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -4467,7 +5824,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="66" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4493,7 +5850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="63" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4519,7 +5876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4545,7 +5902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="75">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4571,7 +5928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="75">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4597,7 +5954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="90">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4623,7 +5980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="60">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4649,7 +6006,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4663,19 +6020,19 @@
         <v>318</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4686,32 +6043,48 @@
         <v>317</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>322</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -4721,7 +6094,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -4731,7 +6104,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="14">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4741,7 +6114,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
@@ -4751,7 +6124,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="14">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
@@ -4761,7 +6134,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="14">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4771,7 +6144,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="14">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4781,7 +6154,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="14">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4791,7 +6164,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="14">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4801,7 +6174,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="14">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4811,7 +6184,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="14">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4821,7 +6194,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="14">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4831,7 +6204,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4841,7 +6214,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="14">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4851,7 +6224,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4861,7 +6234,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4871,7 +6244,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4881,7 +6254,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4891,7 +6264,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4901,7 +6274,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4911,7 +6284,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="14">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4921,7 +6294,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="14">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4931,7 +6304,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="14">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4941,7 +6314,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="14">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4951,7 +6324,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="14">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4961,7 +6334,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4971,7 +6344,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="14">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4981,7 +6354,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="14">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4991,7 +6364,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="14">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5001,7 +6374,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="14">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5011,7 +6384,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="14">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -5021,7 +6394,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="14">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -5031,7 +6404,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="14">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -5041,7 +6414,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="14">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -5051,7 +6424,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="14">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -5061,7 +6434,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="14">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -5071,7 +6444,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="14">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -5081,7 +6454,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="14">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -5091,7 +6464,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="14">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5101,7 +6474,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="14">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5111,7 +6484,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="14">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -5121,7 +6494,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="14">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -5131,7 +6504,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="14">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -5141,7 +6514,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="14">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "JSON testcases updated in excel file"""
This reverts commit b9fe809ba11446e853b94c70a6f78cdf70373a95.
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amey/Documents/GitHub/project-g3t4/testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rou Hui\Documents\GitHub\project-g3t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3213DF3F-6A19-2545-A9E1-8E0E3EF25A9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39E3E23-BA92-47E7-962C-53E42B62672D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1 – Manual – Login Bo" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 1 - JSON - Login" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 1 – JSON – Authentica" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration 2 - Manual - Round 1" sheetId="4" r:id="rId4"/>
-    <sheet name="Iteration 2 -- JSON" sheetId="6" r:id="rId5"/>
-    <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId6"/>
+    <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="324">
   <si>
     <t>S/N</t>
   </si>
@@ -1342,1010 +1341,26 @@
     <t>student bids for section that has 0 vancancies with the minimum bid</t>
   </si>
   <si>
+    <t xml:space="preserve">ben.ong bids e$12 for IS100 </t>
+  </si>
+  <si>
     <t>"Pending, fail"</t>
   </si>
   <si>
     <t>student bids for section that has vacancies with the minimum bid</t>
   </si>
   <si>
+    <t>ben.ong bids for e$14.01 for IS100</t>
+  </si>
+  <si>
     <t>"Pending, successful"</t>
-  </si>
-  <si>
-    <t>ben.ng bids for e$14.01 for IS100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ben.ng bids e$12 for IS100 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 students bid the same amount for one vacancy </t>
-  </si>
-  <si>
-    <t>ben.ng and za.ng bid e$10 for is100</t>
-  </si>
-  <si>
-    <t>both unsucessful</t>
-  </si>
-  <si>
-    <t>error thrown</t>
-  </si>
-  <si>
-    <t>username=calvin.ng.2009</t>
-  </si>
-  <si>
-    <t>username=calvin.ng.2009
-password=qwerty130</t>
-  </si>
-  <si>
-    <t>username=calvin.ng.2009
-password=wrongpasswordhaha</t>
-  </si>
-  <si>
-    <t>EMPTY</t>
-  </si>
-  <si>
-    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS102","section": "S1"}</t>
-  </si>
-  <si>
-    <t>r={"userid": "ada.goh.2012","amount": 11.0,"course": "IS100","section": "S1"}</t>
-  </si>
-  <si>
-    <t>r={"userid": "amy.ng.2009","amount": 9.0,"course": "IS100","section": "S1"}</t>
-  </si>
-  <si>
-    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS110","section": "S1"}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "error",
-    "message": [
-        "round not started"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success",
-    "round": "1"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success",
-    "courses": [
-        {
-            "course": "ECON001",
-            "school": "SOE",
-            "title": "Microeconomics",
-            "description": "Microeconomics is about economics in smaller scale (e.g. firm-scale)",
-            "examdate": "20131101",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "ECON002",
-            "school": "SOE",
-            "title": "Macroeconomics",
-            "description": "You don't learn about excel macros here.",
-            "examdate": "20131101",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS100",
-            "school": "SIS",
-            "title": "Calculus ",
-            "description": "The basic objective of Calculus is to relate small-scale (differential) quantities to large-scale (integrated) quantities. This is accomplished by means of the Fundamental Theorem of Calculus. Students should demonstrate an understanding of the integral as a cumulative sum, of the derivative as a rate of change, and of the inverse relationship between integration and differentiation.",
-            "examdate": "20131119",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS101",
-            "school": "SIS",
-            "title": "Advanced Calculus",
-            "description": "This is a second course on calculus.\u00a0It is more advanced definitely.",
-            "examdate": "20131118",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS102",
-            "school": "SIS",
-            "title": "Java programming",
-            "description": "This course teaches you on Java programming. I love Java definitely.",
-            "examdate": "20131117",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS103",
-            "school": "SIS",
-            "title": "Web Programming",
-            "description": "JSP, Servlets using Tomcat",
-            "examdate": "20131116",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS104",
-            "school": "SIS",
-            "title": "Advanced Programming",
-            "description": "How to write code that nobody can understand",
-            "examdate": "20131115",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS105",
-            "school": "SIS",
-            "title": "Data Structures",
-            "description": "Data structure is a particular way of storing and organizing data in a computer so that it can be used efficiently. Arrays, Lists, Stacks and Trees will be covered.",
-            "examdate": "20131114",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS106",
-            "school": "SIS",
-            "title": "Database Modeling &amp; Design",
-            "description": "Data modeling in software engineering is the process of creating a data model by applying formal data model descriptions using data modeling techniques. ",
-            "examdate": "20131113",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS107",
-            "school": "SIS",
-            "title": "IT Outsourcing",
-            "description": "This course teaches you on how to outsource your programming projects to others.",
-            "examdate": "20131112",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS108",
-            "school": "SIS",
-            "title": "Organization Behaviour",
-            "description": "Organizational Behavior (OB) is the study and application of knowledge about how people, individuals, and groups act in organizations. ",
-            "examdate": "20131111",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS109",
-            "school": "SIS",
-            "title": "Cloud Computing",
-            "description": "Cloud computing is Internet-based computing, whereby shared resources, software and information are provided to computers and other devices on-demand, like the electricity grid.",
-            "examdate": "20131110",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS200",
-            "school": "SIS",
-            "title": "Final Touch",
-            "description": "Learn how eat, dress and talk.",
-            "examdate": "20131109",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS201",
-            "school": "SIS",
-            "title": "Fun with Shell Programming",
-            "description": "Shell scripts are a fundamental part of the UNIX and Linux programming environment.",
-            "examdate": "20131108",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS202",
-            "school": "SIS",
-            "title": "Enterprise integration",
-            "description": "Enterprise integration is a technical field of Enterprise Architecture, which focused on the study of things like system interconnection, electronic data interchange, product data exchange and distributed computing environments, and it's possible other solutions.[1",
-            "examdate": "20131107",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS203",
-            "school": "SIS",
-            "title": "Software Engineering",
-            "description": "The Sleepless Era.",
-            "examdate": "20131106",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS204",
-            "school": "SIS",
-            "title": "Database System Administration",
-            "description": "Database administration is a complex, often thankless chore.",
-            "examdate": "20131105",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS205",
-            "school": "SIS",
-            "title": "All Talk, No Action",
-            "description": "The easiest course of all. We will sit around and talk.",
-            "examdate": "20131104",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS206",
-            "school": "SIS",
-            "title": "Operation Research",
-            "description": "Operations research, also known as operational research, is an interdisciplinary branch of applied mathematics and formal science that uses advanced analytical methods such as mathematical modeling, statistical analysis, and mathematical optimization to arrive at optimal or near-optimal solutions to complex decision-making problems.",
-            "examdate": "20131103",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "IS207",
-            "school": "SIS",
-            "title": "GUI Bloopers",
-            "description": "Common User Interface Design Don'ts and Dos",
-            "examdate": "20131103",
-            "examstart": "15:30:00",
-            "examend": "18:45:00"
-        },
-        {
-            "course": "IS208",
-            "school": "SIS",
-            "title": "Artifical Intelligence",
-            "description": "The science and engineering of making intelligent machine",
-            "examdate": "20131103",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "IS209",
-            "school": "SIS",
-            "title": "Information Storage and Management",
-            "description": "Information storage and management (ISM) - once a relatively straightforward operation -has developed into a highly sophisticated pillar of information technology, requiring proven technical expertise.",
-            "examdate": "20131102",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        },
-        {
-            "course": "MGMT001",
-            "school": "SOB",
-            "title": "Business,Government, and Society",
-            "description": "learn the interrelation amongst the three",
-            "examdate": "20131102",
-            "examstart": "08:30:00",
-            "examend": "11:45:00"
-        },
-        {
-            "course": "MGMT002",
-            "school": "SOB",
-            "title": "Technology and World Change",
-            "description": "As technology changes, so does the world",
-            "examdate": "20131101",
-            "examstart": "12:00:00",
-            "examend": "15:15:00"
-        }
-    ],
-    "section": [
-        {
-            "course": "ECON001",
-            "section": "S1",
-            "day": "4",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "John KHOO",
-            "venue": "Seminar Rm 2-34",
-            "size": "10"
-        },
-        {
-            "course": "ECON002",
-            "section": "S1",
-            "day": "5",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Andy KHOO",
-            "venue": "Seminar Rm 2-35",
-            "size": "10"
-        },
-        {
-            "course": "IS100",
-            "section": "S1",
-            "day": "1",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Albert KHOO",
-            "venue": "Seminar Rm 2-1",
-            "size": "10"
-        },
-        {
-            "course": "IS100",
-            "section": "S2",
-            "day": "2",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Billy KHOO",
-            "venue": "Seminar Rm 2-2",
-            "size": "10"
-        },
-        {
-            "course": "IS101",
-            "section": "S1",
-            "day": "3",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Cheri KHOO",
-            "venue": "Seminar Rm 2-3",
-            "size": "10"
-        },
-        {
-            "course": "IS101",
-            "section": "S2",
-            "day": "4",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Daniel KHOO",
-            "venue": "Seminar Rm 2-4",
-            "size": "10"
-        },
-        {
-            "course": "IS101",
-            "section": "S3",
-            "day": "5",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Ernest KHOO",
-            "venue": "Seminar Rm 2-5",
-            "size": "10"
-        },
-        {
-            "course": "IS102",
-            "section": "S1",
-            "day": "1",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Felicia KHOO",
-            "venue": "Seminar Rm 2-6",
-            "size": "10"
-        },
-        {
-            "course": "IS102",
-            "section": "S2",
-            "day": "2",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Gerald KHOO",
-            "venue": "Seminar Rm 2-7",
-            "size": "10"
-        },
-        {
-            "course": "IS102",
-            "section": "S3",
-            "day": "3",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Henry KHOO",
-            "venue": "Seminar Rm 2-8",
-            "size": "10"
-        },
-        {
-            "course": "IS103",
-            "section": "S1",
-            "day": "4",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Ivy KHOO",
-            "venue": "Seminar Rm 2-9",
-            "size": "10"
-        },
-        {
-            "course": "IS103",
-            "section": "S2",
-            "day": "5",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Jason KHOO",
-            "venue": "Seminar Rm 2-10",
-            "size": "10"
-        },
-        {
-            "course": "IS103",
-            "section": "S3",
-            "day": "1",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Kat KHOO",
-            "venue": "Seminar Rm 2-11",
-            "size": "10"
-        },
-        {
-            "course": "IS104",
-            "section": "S1",
-            "day": "2",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Linn KHOO",
-            "venue": "Seminar Rm 2-12",
-            "size": "10"
-        },
-        {
-            "course": "IS104",
-            "section": "S2",
-            "day": "3",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Michael KHOO",
-            "venue": "Seminar Rm 2-13",
-            "size": "10"
-        },
-        {
-            "course": "IS105",
-            "section": "S1",
-            "day": "4",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Nathaniel KHOO",
-            "venue": "Seminar Rm 2-14",
-            "size": "10"
-        },
-        {
-            "course": "IS105",
-            "section": "S2",
-            "day": "5",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Oreilly KHOO",
-            "venue": "Seminar Rm 2-15",
-            "size": "10"
-        },
-        {
-            "course": "IS106",
-            "section": "S1",
-            "day": "1",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Peter KHOO",
-            "venue": "Seminar Rm 2-16",
-            "size": "10"
-        },
-        {
-            "course": "IS106",
-            "section": "S2",
-            "day": "2",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Queen KHOO",
-            "venue": "Seminar Rm 2-17",
-            "size": "10"
-        },
-        {
-            "course": "IS107",
-            "section": "S1",
-            "day": "3",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Ray KHOO",
-            "venue": "Seminar Rm 2-18",
-            "size": "10"
-        },
-        {
-            "course": "IS107",
-            "section": "S2",
-            "day": "4",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Simon KHOO",
-            "venue": "Seminar Rm 2-19",
-            "size": "10"
-        },
-        {
-            "course": "IS108",
-            "section": "S1",
-            "day": "5",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Tim KHOO",
-            "venue": "Seminar Rm 2-20",
-            "size": "10"
-        },
-        {
-            "course": "IS109",
-            "section": "S1",
-            "day": "2",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Vincent KHOO",
-            "venue": "Seminar Rm 2-22",
-            "size": "10"
-        },
-        {
-            "course": "IS109",
-            "section": "S2",
-            "day": "3",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Winnie KHOO",
-            "venue": "Seminar Rm 2-23",
-            "size": "10"
-        },
-        {
-            "course": "IS200",
-            "section": "S1",
-            "day": "4",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Xtra KHOO",
-            "venue": "Seminar Rm 2-24",
-            "size": "10"
-        },
-        {
-            "course": "IS201",
-            "section": "S1",
-            "day": "5",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Yale KHOO",
-            "venue": "Seminar Rm 2-25",
-            "size": "10"
-        },
-        {
-            "course": "IS202",
-            "section": "S1",
-            "day": "1",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Zen KHOO",
-            "venue": "Seminar Rm 2-26",
-            "size": "10"
-        },
-        {
-            "course": "IS203",
-            "section": "S1",
-            "day": "2",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Anderson KHOO",
-            "venue": "Seminar Rm 2-27",
-            "size": "10"
-        },
-        {
-            "course": "IS204",
-            "section": "S1",
-            "day": "3",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Bing KHOO",
-            "venue": "Seminar Rm 2-28",
-            "size": "10"
-        },
-        {
-            "course": "IS205",
-            "section": "S1",
-            "day": "4",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Carlo KHOO",
-            "venue": "Seminar Rm 2-29",
-            "size": "10"
-        },
-        {
-            "course": "IS206",
-            "section": "S1",
-            "day": "5",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Dickson KHOO",
-            "venue": "Seminar Rm 2-30",
-            "size": "10"
-        },
-        {
-            "course": "IS207",
-            "section": "S1",
-            "day": "1",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Edmund KHOO",
-            "venue": "Seminar Rm 2-31",
-            "size": "10"
-        },
-        {
-            "course": "IS208",
-            "section": "S1",
-            "day": "2",
-            "start": "12:00:00",
-            "end": "15:15:00",
-            "instructor": "Febrice KHOO",
-            "venue": "Seminar Rm 2-32",
-            "size": "10"
-        },
-        {
-            "course": "MGMT001",
-            "section": "S1",
-            "day": "3",
-            "start": "08:30:00",
-            "end": "11:45:00",
-            "instructor": "Gavin KHOO",
-            "venue": "Seminar Rm 2-33",
-            "size": "10"
-        },
-        {
-            "course": "MGMT002",
-            "section": "S1",
-            "day": "3",
-            "start": "15:30:00",
-            "end": "18:45:00",
-            "instructor": "Bob KHOO",
-            "venue": "Seminar Rm 2-37",
-            "size": "10"
-        }
-    ],
-    "students": [
-        {
-            "userid": "amy.ng.2009",
-            "password": "qwerty128",
-            "name": "Amy NG",
-            "school": "SIS",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "ben.ng.2009",
-            "password": "qwerty129",
-            "name": "Ben NG",
-            "school": "SIS",
-            "edollar": "189.00"
-        },
-        {
-            "userid": "calvin.ng.2009",
-            "password": "qwerty130",
-            "name": "Calvin NG",
-            "school": "SIS",
-            "edollar": "188.00"
-        },
-        {
-            "userid": "dawn.ng.2009",
-            "password": "qwerty131",
-            "name": "Dawn NG",
-            "school": "SIS",
-            "edollar": "187.00"
-        },
-        {
-            "userid": "eddy.ng.2009",
-            "password": "qwerty132",
-            "name": "Eddy NG",
-            "school": "SIS",
-            "edollar": "186.00"
-        },
-        {
-            "userid": "fred.ng.2009",
-            "password": "qwerty133",
-            "name": "Fred NG",
-            "school": "SIS",
-            "edollar": "185.00"
-        },
-        {
-            "userid": "gary.ng.2009",
-            "password": "qwerty134",
-            "name": "Gary NG",
-            "school": "SIS",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "harry.ng.2009",
-            "password": "qwerty135",
-            "name": "Harry NG",
-            "school": "SIS",
-            "edollar": "183.00"
-        },
-        {
-            "userid": "ian.ng.2009",
-            "password": "qwerty136",
-            "name": "Ian NG",
-            "school": "SIS",
-            "edollar": "182.00"
-        },
-        {
-            "userid": "jerry.ng.2009",
-            "password": "qwerty137",
-            "name": "Jerry NG",
-            "school": "SIS",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "kelly.ng.2009",
-            "password": "qwerty138",
-            "name": "Kelly NG",
-            "school": "SIS",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "larry.ng.2009",
-            "password": "qwerty139",
-            "name": "Larry NG",
-            "school": "SIS",
-            "edollar": "181.00"
-        },
-        {
-            "userid": "maggie.ng.2009",
-            "password": "qwerty140",
-            "name": "Maggie NG",
-            "school": "SIS",
-            "edollar": "180.00"
-        },
-        {
-            "userid": "neilson.ng.2009",
-            "password": "qwerty141",
-            "name": "Neilson NG",
-            "school": "SIS",
-            "edollar": "179.00"
-        },
-        {
-            "userid": "olivia.ng.2009",
-            "password": "qwerty142",
-            "name": "Olivia NG",
-            "school": "SIS",
-            "edollar": "178.00"
-        },
-        {
-            "userid": "parker.ng.2009",
-            "password": "qwerty143",
-            "name": "Parker NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "quiten.ng.2009",
-            "password": "qwerty144",
-            "name": "Quiten NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "ricky.ng.2009",
-            "password": "qwerty145",
-            "name": "Ricky NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "steven.ng.2009",
-            "password": "qwerty146",
-            "name": "Steven NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "timothy.ng.2009",
-            "password": "qwerty147",
-            "name": "Timothy NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "ursala.ng.2009",
-            "password": "qwerty148",
-            "name": "Ursala NG",
-            "school": "SOE",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "valarie.ng.2009",
-            "password": "qwerty149",
-            "name": "Valarie NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "winston.ng.2009",
-            "password": "qwerty150",
-            "name": "Winston NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "xavier.ng.2009",
-            "password": "qwerty151",
-            "name": "Xavier NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "yasir.ng.2009",
-            "password": "qwerty152",
-            "name": "Yasir NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        },
-        {
-            "userid": "zac.ng.2009",
-            "password": "qwerty153",
-            "name": "Zac NG",
-            "school": "SOB",
-            "edollar": "200.00"
-        }
-    ],
-    "prerequisite": [
-        {
-            "course": "IS101",
-            "prerequisite": "IS100"
-        },
-        {
-            "course": "IS103",
-            "prerequisite": "IS102"
-        },
-        {
-            "course": "IS104",
-            "prerequisite": "IS103"
-        },
-        {
-            "course": "IS109",
-            "prerequisite": "IS102"
-        },
-        {
-            "course": "IS203",
-            "prerequisite": "IS103"
-        },
-        {
-            "course": "IS203",
-            "prerequisite": "IS106"
-        },
-        {
-            "course": "IS204",
-            "prerequisite": "IS106"
-        },
-        {
-            "course": "IS209",
-            "prerequisite": "IS106"
-        }
-    ],
-    "bid": [
-        {
-            "userid": "olivia.ng.2009",
-            "amount": "22.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "neilson.ng.2009",
-            "amount": "21.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "maggie.ng.2009",
-            "amount": "20.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "larry.ng.2009",
-            "amount": "19.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "ian.ng.2009",
-            "amount": "18.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "harry.ng.2009",
-            "amount": "17.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "fred.ng.2009",
-            "amount": "15.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "eddy.ng.2009",
-            "amount": "14.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "dawn.ng.2009",
-            "amount": "13.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "calvin.ng.2009",
-            "amount": "12.00",
-            "course": "IS100",
-            "section": "S1"
-        },
-        {
-            "userid": "ben.ng.2009",
-            "amount": "11.00",
-            "course": "IS100",
-            "section": "S1"
-        }
-    ],
-    "completed-course": [
-        {
-            "userid": "amy.ng.2009",
-            "course": "IS100"
-        },
-        {
-            "userid": "gary.ng.2009",
-            "course": "IS100"
-        },
-        {
-            "userid": "ben.ng.2009",
-            "course": "IS102"
-        },
-        {
-            "userid": "ben.ng.2009",
-            "course": "IS103"
-        }
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "error",
-    "message": [
-        "invalid userid"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>Authentication</t>
-  </si>
-  <si>
-    <t>Stop round</t>
-  </si>
-  <si>
-    <t>Start round</t>
-  </si>
-  <si>
-    <t>Dump</t>
-  </si>
-  <si>
-    <t>{
-    "status": "error",
-    "message": [
-        "invalid amount"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "error",
-    "message": [
-        "invalid course"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>Update bid - succesful case</t>
-  </si>
-  <si>
-    <t>Update bid - enter invalid user</t>
-  </si>
-  <si>
-    <t>Update bid - enter invalid amount</t>
-  </si>
-  <si>
-    <t>Update bid - enter invalid course</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2735,16 +1750,16 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
+    <row r="1" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2770,7 +1785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2780,7 +1795,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="60">
+    <row r="3" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2806,7 +1821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="75">
+    <row r="4" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2832,7 +1847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60">
+    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2858,7 +1873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60">
+    <row r="6" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2884,7 +1899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60">
+    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2910,7 +1925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45">
+    <row r="8" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2936,7 +1951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45">
+    <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2962,7 +1977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60">
+    <row r="10" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2988,7 +2003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3014,7 +2029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3040,7 +2055,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3066,7 +2081,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="120">
+    <row r="14" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -3092,7 +2107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="120">
+    <row r="15" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -3118,7 +2133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -3144,7 +2159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45">
+    <row r="17" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -3170,7 +2185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -3196,7 +2211,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="75">
+    <row r="19" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -3222,7 +2237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45">
+    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -3248,7 +2263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="120">
+    <row r="21" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -3274,7 +2289,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45">
+    <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -3300,7 +2315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="45">
+    <row r="23" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -3326,7 +2341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45">
+    <row r="24" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -3352,7 +2367,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45">
+    <row r="25" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -3378,7 +2393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45">
+    <row r="26" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -3404,7 +2419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="60">
+    <row r="27" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -3430,7 +2445,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45">
+    <row r="28" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -3456,7 +2471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="105">
+    <row r="29" spans="1:8" ht="98" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -3482,7 +2497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="409.6">
+    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -3508,7 +2523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="225">
+    <row r="31" spans="1:8" ht="224" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -3534,7 +2549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="45">
+    <row r="32" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -3560,7 +2575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45">
+    <row r="33" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -3586,7 +2601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="45">
+    <row r="34" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -3612,7 +2627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="45">
+    <row r="35" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -3638,7 +2653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="45">
+    <row r="36" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -3664,7 +2679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="45">
+    <row r="37" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -3690,7 +2705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="60">
+    <row r="38" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -3716,7 +2731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="45">
+    <row r="39" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -3742,7 +2757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="105">
+    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -3768,7 +2783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="105">
+    <row r="41" spans="1:8" ht="98" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -3794,7 +2809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="45">
+    <row r="42" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -3820,7 +2835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="45">
+    <row r="43" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -3846,7 +2861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="165">
+    <row r="44" spans="1:8" ht="154" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -3872,7 +2887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="60">
+    <row r="45" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -3898,7 +2913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="60">
+    <row r="46" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -3924,7 +2939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="45">
+    <row r="47" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -3950,7 +2965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="60">
+    <row r="48" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -3976,7 +2991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="60">
+    <row r="49" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -4002,7 +3017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45">
+    <row r="50" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -4028,7 +3043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="45">
+    <row r="51" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -4054,7 +3069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="45">
+    <row r="52" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -4080,7 +3095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="45">
+    <row r="53" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -4106,7 +3121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="45">
+    <row r="54" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -4132,7 +3147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="60">
+    <row r="55" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -4158,7 +3173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="60">
+    <row r="56" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -4206,20 +3221,20 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.5" customWidth="1"/>
-    <col min="4" max="4" width="78.5" customWidth="1"/>
-    <col min="5" max="5" width="78.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="78.453125" customWidth="1"/>
+    <col min="5" max="5" width="78.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4239,7 +3254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" customHeight="1">
+    <row r="2" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -4247,7 +3262,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="105">
+    <row r="3" spans="1:6" ht="98" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -4267,7 +3282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60">
+    <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -4287,7 +3302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60">
+    <row r="5" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -4307,7 +3322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60">
+    <row r="6" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -4348,17 +3363,17 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="33.6328125" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4378,7 +3393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1">
+    <row r="2" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -4386,7 +3401,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="180">
+    <row r="3" spans="1:6" ht="168" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -4406,7 +3421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.6">
+    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -4447,16 +3462,16 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4482,7 +3497,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -4492,7 +3507,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1">
+    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4518,7 +3533,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1">
+    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4544,7 +3559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4570,7 +3585,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45">
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4596,7 +3611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45">
+    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4622,7 +3637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45">
+    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4648,7 +3663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60">
+    <row r="9" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4674,7 +3689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="75">
+    <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4700,7 +3715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="75">
+    <row r="11" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4726,7 +3741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="75">
+    <row r="12" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4752,7 +3767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4778,7 +3793,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45">
+    <row r="14" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4804,7 +3819,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30">
+    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4830,7 +3845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="75">
+    <row r="16" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4856,7 +3871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="75">
+    <row r="17" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4882,7 +3897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4908,7 +3923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45">
+    <row r="19" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4934,7 +3949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60">
+    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4960,7 +3975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45">
+    <row r="21" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4986,7 +4001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45">
+    <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5012,7 +4027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="75">
+    <row r="23" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -5038,7 +4053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30">
+    <row r="24" spans="1:8" ht="28" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -5064,7 +4079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14">
+    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5074,7 +4089,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14">
+    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5084,7 +4099,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14">
+    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5094,7 +4109,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14">
+    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5104,7 +4119,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14">
+    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5114,7 +4129,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14">
+    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5124,7 +4139,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14">
+    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5134,7 +4149,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14">
+    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5144,7 +4159,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14">
+    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5154,7 +4169,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14">
+    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5164,7 +4179,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14">
+    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5174,7 +4189,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14">
+    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5184,7 +4199,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14">
+    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5194,7 +4209,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14">
+    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5204,7 +4219,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14">
+    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -5214,7 +4229,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14">
+    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -5224,7 +4239,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14">
+    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5234,7 +4249,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14">
+    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5244,7 +4259,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14">
+    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -5254,7 +4269,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14">
+    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -5264,7 +4279,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14">
+    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -5274,7 +4289,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14">
+    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -5284,7 +4299,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14">
+    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -5294,7 +4309,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14">
+    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -5304,7 +4319,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14">
+    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -5314,7 +4329,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14">
+    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -5324,7 +4339,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14">
+    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5334,7 +4349,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14">
+    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5344,7 +4359,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14">
+    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -5354,7 +4369,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14">
+    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -5364,7 +4379,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14">
+    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -5374,7 +4389,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14">
+    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
@@ -5400,395 +4415,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED20DAA-AFB2-5240-A261-8BB8E5918D09}">
-  <dimension ref="A1:F22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
-  <cols>
-    <col min="3" max="3" width="30.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" ht="150">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="64" customHeight="1">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="77" customHeight="1">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="90">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="409.6">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="52" customHeight="1">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="90">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="90">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="90">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="14">
-      <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="14">
-      <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="14">
-      <c r="A20" s="2">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="14">
-      <c r="A21" s="2">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="14">
-      <c r="A22" s="2">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA8D5A-5628-41F0-8C3D-F219DADB62EC}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5814,7 +4457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -5824,7 +4467,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1">
+    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5850,7 +4493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1">
+    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5876,7 +4519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45">
+    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5902,7 +4545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="75">
+    <row r="6" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5928,7 +4571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75">
+    <row r="7" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5954,7 +4597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="90">
+    <row r="8" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5980,7 +4623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60">
+    <row r="9" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6006,7 +4649,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45">
+    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6020,19 +4663,19 @@
         <v>318</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6043,48 +4686,32 @@
         <v>317</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>322</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="14">
+    <row r="12" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -6094,7 +4721,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="14">
+    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -6104,7 +4731,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14">
+    <row r="15" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -6114,7 +4741,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="14">
+    <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
@@ -6124,7 +4751,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="14">
+    <row r="17" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
@@ -6134,7 +4761,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="14">
+    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6144,7 +4771,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="14">
+    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6154,7 +4781,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="14">
+    <row r="20" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6164,7 +4791,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="14">
+    <row r="21" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6174,7 +4801,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="14">
+    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6184,7 +4811,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="14">
+    <row r="23" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6194,7 +4821,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="14">
+    <row r="24" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6204,7 +4831,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="14">
+    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6214,7 +4841,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14">
+    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6224,7 +4851,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14">
+    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6234,7 +4861,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14">
+    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6244,7 +4871,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14">
+    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6254,7 +4881,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14">
+    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6264,7 +4891,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14">
+    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6274,7 +4901,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14">
+    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6284,7 +4911,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14">
+    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6294,7 +4921,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14">
+    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6304,7 +4931,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14">
+    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6314,7 +4941,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14">
+    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -6324,7 +4951,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14">
+    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6334,7 +4961,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14">
+    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6344,7 +4971,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14">
+    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -6354,7 +4981,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14">
+    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -6364,7 +4991,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14">
+    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -6374,7 +5001,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14">
+    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -6384,7 +5011,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14">
+    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -6394,7 +5021,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14">
+    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -6404,7 +5031,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14">
+    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -6414,7 +5041,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14">
+    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -6424,7 +5051,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14">
+    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -6434,7 +5061,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14">
+    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -6444,7 +5071,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14">
+    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -6454,7 +5081,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14">
+    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -6464,7 +5091,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14">
+    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -6474,7 +5101,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14">
+    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -6484,7 +5111,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14">
+    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6494,7 +5121,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14">
+    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -6504,7 +5131,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14">
+    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -6514,7 +5141,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14">
+    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>

</xml_diff>

<commit_message>
Updated testcases.xlsx for JSON testcase
updated iteration 2 JSON testcases
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amey/Documents/GitHub/project-g3t4/testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rou Hui\Documents\GitHub\project-g3t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3213DF3F-6A19-2545-A9E1-8E0E3EF25A9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B54332-F369-4206-AB12-54C778ADD5C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1 – Manual – Login Bo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="393">
   <si>
     <t>S/N</t>
   </si>
@@ -2340,12 +2340,282 @@
   <si>
     <t>Update bid - enter invalid course</t>
   </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","amount": 11.0,"course": "IS100","section": "S3"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "ada.goh.2012","course": "IS100","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","course": "IS110","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","course": "IS102","section": "S4"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","course": "IS102","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","course": "IS100","section": "S3"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","course": "IS100","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "ada.goh.2012"}</t>
+  </si>
+  <si>
+    <t>r={"course": "IS100","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"course": "IS110","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"course": "IS100","section": "S3"}</t>
+  </si>
+  <si>
+    <t>round=2</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid section"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "no such bid"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "no such enrollment found"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "userid": "amy.ng.2009",
+    "password": "qwerty128",
+    "name": "Amy NG",
+    "school": "SIS",
+    "edollar": "211.00"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "bids": [
+        {
+            "row": 1,
+            "userid": "olivia.ng.2009",
+            "amount": "22.00",
+            "result": "-"
+        },
+        {
+            "row": 2,
+            "userid": "neilson.ng.2009",
+            "amount": "21.00",
+            "result": "-"
+        },
+        {
+            "row": 3,
+            "userid": "maggie.ng.2009",
+            "amount": "20.00",
+            "result": "-"
+        },
+        {
+            "row": 4,
+            "userid": "larry.ng.2009",
+            "amount": "19.00",
+            "result": "-"
+        },
+        {
+            "row": 5,
+            "userid": "ian.ng.2009",
+            "amount": "18.00",
+            "result": "-"
+        },
+        {
+            "row": 6,
+            "userid": "harry.ng.2009",
+            "amount": "17.00",
+            "result": "-"
+        },
+        {
+            "row": 7,
+            "userid": "fred.ng.2009",
+            "amount": "15.00",
+            "result": "-"
+        },
+        {
+            "row": 8,
+            "userid": "eddy.ng.2009",
+            "amount": "14.00",
+            "result": "-"
+        },
+        {
+            "row": 9,
+            "userid": "dawn.ng.2009",
+            "amount": "13.00",
+            "result": "-"
+        },
+        {
+            "row": 10,
+            "userid": "calvin.ng.2009",
+            "amount": "12.00",
+            "result": "-"
+        },
+        {
+            "row": 11,
+            "userid": "ben.ng.2009",
+            "amount": "11.00",
+            "result": "-"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "students": [
+        {
+            "userid": "calvin.ng.2009",
+            "amount": "12.00"
+        },
+        {
+            "userid": "dawn.ng.2009",
+            "amount": "13.00"
+        },
+        {
+            "userid": "eddy.ng.2009",
+            "amount": "14.00"
+        },
+        {
+            "userid": "fred.ng.2009",
+            "amount": "15.00"
+        },
+        {
+            "userid": "harry.ng.2009",
+            "amount": "17.00"
+        },
+        {
+            "userid": "ian.ng.2009",
+            "amount": "18.00"
+        },
+        {
+            "userid": "larry.ng.2009",
+            "amount": "19.00"
+        },
+        {
+            "userid": "maggie.ng.2009",
+            "amount": "20.00"
+        },
+        {
+            "userid": "neilson.ng.2009",
+            "amount": "21.00"
+        },
+        {
+            "userid": "olivia.ng.2009",
+            "amount": "22.00"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "round already ended"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "round": 2
+}</t>
+  </si>
+  <si>
+    <t>Update bid - invalid section</t>
+  </si>
+  <si>
+    <t>Delete bid - invalid userid</t>
+  </si>
+  <si>
+    <t>Delete bid - invalid course</t>
+  </si>
+  <si>
+    <t>Delete bid - invalid section</t>
+  </si>
+  <si>
+    <t>Delete bid - success</t>
+  </si>
+  <si>
+    <t>Delete bid - no such bid</t>
+  </si>
+  <si>
+    <t>Drop section - invalid userid</t>
+  </si>
+  <si>
+    <t>Drop section - invalid course</t>
+  </si>
+  <si>
+    <t>Drop section - invalid section</t>
+  </si>
+  <si>
+    <t>Drop section - success</t>
+  </si>
+  <si>
+    <t>Drop section - no such enrollment found</t>
+  </si>
+  <si>
+    <t>User dump - success</t>
+  </si>
+  <si>
+    <t>User dump - error</t>
+  </si>
+  <si>
+    <t>Bid dump - success</t>
+  </si>
+  <si>
+    <t>Bid dump - invalid course</t>
+  </si>
+  <si>
+    <t>Bid dump - invalid section</t>
+  </si>
+  <si>
+    <t>Stop round 1</t>
+  </si>
+  <si>
+    <t>Section dump - success</t>
+  </si>
+  <si>
+    <t>Section dump - invalid course</t>
+  </si>
+  <si>
+    <t>Section dump - invalid section</t>
+  </si>
+  <si>
+    <t>Start round 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2735,16 +3005,16 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
+    <row r="1" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2770,7 +3040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2780,7 +3050,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="60">
+    <row r="3" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2806,7 +3076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="75">
+    <row r="4" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2832,7 +3102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60">
+    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2858,7 +3128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60">
+    <row r="6" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2884,7 +3154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60">
+    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2910,7 +3180,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45">
+    <row r="8" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2936,7 +3206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45">
+    <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2962,7 +3232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60">
+    <row r="10" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2988,7 +3258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3014,7 +3284,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3040,7 +3310,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3066,7 +3336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="120">
+    <row r="14" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -3092,7 +3362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="120">
+    <row r="15" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -3118,7 +3388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -3144,7 +3414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45">
+    <row r="17" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -3170,7 +3440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -3196,7 +3466,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="75">
+    <row r="19" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -3222,7 +3492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45">
+    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -3248,7 +3518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="120">
+    <row r="21" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -3274,7 +3544,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45">
+    <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -3300,7 +3570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="45">
+    <row r="23" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -3326,7 +3596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45">
+    <row r="24" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -3352,7 +3622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45">
+    <row r="25" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -3378,7 +3648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45">
+    <row r="26" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -3404,7 +3674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="60">
+    <row r="27" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -3430,7 +3700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45">
+    <row r="28" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -3456,7 +3726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="105">
+    <row r="29" spans="1:8" ht="98" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -3482,7 +3752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="409.6">
+    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -3508,7 +3778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="225">
+    <row r="31" spans="1:8" ht="224" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -3534,7 +3804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="45">
+    <row r="32" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -3560,7 +3830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45">
+    <row r="33" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -3586,7 +3856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="45">
+    <row r="34" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -3612,7 +3882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="45">
+    <row r="35" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -3638,7 +3908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="45">
+    <row r="36" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -3664,7 +3934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="45">
+    <row r="37" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -3690,7 +3960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="60">
+    <row r="38" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -3716,7 +3986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="45">
+    <row r="39" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -3742,7 +4012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="105">
+    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -3768,7 +4038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="105">
+    <row r="41" spans="1:8" ht="98" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -3794,7 +4064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="45">
+    <row r="42" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -3820,7 +4090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="45">
+    <row r="43" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -3846,7 +4116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="165">
+    <row r="44" spans="1:8" ht="154" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -3872,7 +4142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="60">
+    <row r="45" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -3898,7 +4168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="60">
+    <row r="46" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -3924,7 +4194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="45">
+    <row r="47" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -3950,7 +4220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="60">
+    <row r="48" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -3976,7 +4246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="60">
+    <row r="49" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -4002,7 +4272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45">
+    <row r="50" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -4028,7 +4298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="45">
+    <row r="51" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -4054,7 +4324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="45">
+    <row r="52" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -4080,7 +4350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="45">
+    <row r="53" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -4106,7 +4376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="45">
+    <row r="54" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -4132,7 +4402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="60">
+    <row r="55" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -4158,7 +4428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="60">
+    <row r="56" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -4210,16 +4480,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.5" customWidth="1"/>
-    <col min="4" max="4" width="78.5" customWidth="1"/>
-    <col min="5" max="5" width="78.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="78.453125" customWidth="1"/>
+    <col min="5" max="5" width="78.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4239,7 +4509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" customHeight="1">
+    <row r="2" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -4247,7 +4517,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="105">
+    <row r="3" spans="1:6" ht="98" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -4267,7 +4537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60">
+    <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -4287,7 +4557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60">
+    <row r="5" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -4307,7 +4577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60">
+    <row r="6" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -4351,14 +4621,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="33.6328125" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4378,7 +4648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1">
+    <row r="2" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -4386,7 +4656,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="180">
+    <row r="3" spans="1:6" ht="168" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -4406,7 +4676,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.6">
+    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -4447,16 +4717,16 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4482,7 +4752,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -4492,7 +4762,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1">
+    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4518,7 +4788,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1">
+    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4544,7 +4814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4570,7 +4840,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45">
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4596,7 +4866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45">
+    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4622,7 +4892,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45">
+    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4648,7 +4918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60">
+    <row r="9" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4674,7 +4944,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="75">
+    <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4700,7 +4970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="75">
+    <row r="11" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4726,7 +4996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="75">
+    <row r="12" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4752,7 +5022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4778,7 +5048,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45">
+    <row r="14" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4804,7 +5074,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30">
+    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4830,7 +5100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="75">
+    <row r="16" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4856,7 +5126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="75">
+    <row r="17" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4882,7 +5152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4908,7 +5178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45">
+    <row r="19" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4934,7 +5204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60">
+    <row r="20" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4960,7 +5230,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45">
+    <row r="21" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4986,7 +5256,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45">
+    <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5012,7 +5282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="75">
+    <row r="23" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -5038,7 +5308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30">
+    <row r="24" spans="1:8" ht="28" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -5064,7 +5334,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14">
+    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5074,7 +5344,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14">
+    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5084,7 +5354,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14">
+    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5094,7 +5364,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14">
+    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5104,7 +5374,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14">
+    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5114,7 +5384,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14">
+    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5124,7 +5394,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14">
+    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5134,7 +5404,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14">
+    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5144,7 +5414,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14">
+    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5154,7 +5424,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14">
+    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5164,7 +5434,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14">
+    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5174,7 +5444,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14">
+    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5184,7 +5454,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14">
+    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5194,7 +5464,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14">
+    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5204,7 +5474,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14">
+    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -5214,7 +5484,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14">
+    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -5224,7 +5494,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14">
+    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5234,7 +5504,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14">
+    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5244,7 +5514,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14">
+    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -5254,7 +5524,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14">
+    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -5264,7 +5534,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14">
+    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -5274,7 +5544,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14">
+    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -5284,7 +5554,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14">
+    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -5294,7 +5564,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14">
+    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -5304,7 +5574,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14">
+    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -5314,7 +5584,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14">
+    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -5324,7 +5594,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14">
+    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5334,7 +5604,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14">
+    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5344,7 +5614,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14">
+    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -5354,7 +5624,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14">
+    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -5364,7 +5634,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14">
+    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -5374,7 +5644,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14">
+    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
@@ -5401,20 +5671,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED20DAA-AFB2-5240-A261-8BB8E5918D09}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="76" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="33.6328125" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -5434,7 +5704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="48" customHeight="1">
+    <row r="2" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -5442,7 +5712,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="150">
+    <row r="3" spans="1:6" ht="140" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -5462,7 +5732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="64" customHeight="1">
+    <row r="4" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -5482,7 +5752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="77" customHeight="1">
+    <row r="5" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -5502,7 +5772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="75">
+    <row r="6" spans="1:6" ht="70" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -5522,7 +5792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="90">
+    <row r="7" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -5542,7 +5812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60">
+    <row r="8" spans="1:6" ht="56" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -5562,7 +5832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="409.6">
+    <row r="9" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -5580,7 +5850,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="52" customHeight="1">
+    <row r="10" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -5600,7 +5870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="90">
+    <row r="11" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -5620,7 +5890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="90">
+    <row r="12" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -5640,7 +5910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="90">
+    <row r="13" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -5660,112 +5930,454 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15">
+    <row r="14" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="F14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15">
+    <row r="15" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>340</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>346</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15">
+    <row r="17" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="F17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="14">
+      <c r="B18" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="14">
+      <c r="B19" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="14">
+      <c r="B20" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="14">
+      <c r="B21" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="42" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="84" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="112" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="84" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="84" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="84" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="42" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="84" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="84" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="84" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5779,16 +6391,16 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5814,7 +6426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1">
+    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -5824,7 +6436,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1">
+    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5850,7 +6462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1">
+    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5876,7 +6488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45">
+    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5902,7 +6514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="75">
+    <row r="6" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5928,7 +6540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75">
+    <row r="7" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5954,7 +6566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="90">
+    <row r="8" spans="1:8" ht="84" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5980,7 +6592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60">
+    <row r="9" spans="1:8" ht="70" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6006,7 +6618,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45">
+    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6032,7 +6644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6058,7 +6670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6084,7 +6696,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14">
+    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -6094,7 +6706,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="14">
+    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -6104,7 +6716,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14">
+    <row r="15" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -6114,7 +6726,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="14">
+    <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
@@ -6124,7 +6736,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="14">
+    <row r="17" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
@@ -6134,7 +6746,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="14">
+    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6144,7 +6756,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="14">
+    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6154,7 +6766,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="14">
+    <row r="20" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6164,7 +6776,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="14">
+    <row r="21" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6174,7 +6786,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="14">
+    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6184,7 +6796,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="14">
+    <row r="23" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6194,7 +6806,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="14">
+    <row r="24" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6204,7 +6816,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="14">
+    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6214,7 +6826,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="14">
+    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6224,7 +6836,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="14">
+    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6234,7 +6846,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="14">
+    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6244,7 +6856,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="14">
+    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6254,7 +6866,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="14">
+    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6264,7 +6876,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="14">
+    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6274,7 +6886,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="14">
+    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6284,7 +6896,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="14">
+    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6294,7 +6906,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="14">
+    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6304,7 +6916,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="14">
+    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6314,7 +6926,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="14">
+    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -6324,7 +6936,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="14">
+    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6334,7 +6946,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="14">
+    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6344,7 +6956,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="14">
+    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -6354,7 +6966,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="14">
+    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -6364,7 +6976,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="14">
+    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -6374,7 +6986,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="14">
+    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -6384,7 +6996,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="14">
+    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -6394,7 +7006,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="14">
+    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -6404,7 +7016,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="14">
+    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -6414,7 +7026,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="14">
+    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -6424,7 +7036,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="14">
+    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -6434,7 +7046,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="14">
+    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -6444,7 +7056,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" ht="14">
+    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -6454,7 +7066,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" ht="14">
+    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -6464,7 +7076,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14">
+    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -6474,7 +7086,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" ht="14">
+    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -6484,7 +7096,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" ht="14">
+    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6494,7 +7106,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" ht="14">
+    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -6504,7 +7116,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="14">
+    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -6514,7 +7126,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" ht="14">
+    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>

</xml_diff>

<commit_message>
Added iter 3 test cases
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rou Hui\Documents\GitHub\project-g3t4\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g3t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B54332-F369-4206-AB12-54C778ADD5C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B351C513-8009-4E15-AC5C-47082BB03A4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1 – Manual – Login Bo" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="Iteration 2 - Manual - Round 1" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration 2 -- JSON" sheetId="6" r:id="rId5"/>
     <sheet name="Iteration 2 - Manual - Round 2" sheetId="5" r:id="rId6"/>
+    <sheet name="Iteration 3 - Manual -Timetable" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="416">
   <si>
     <t>S/N</t>
   </si>
@@ -2610,12 +2611,81 @@
   <si>
     <t>Start round 2</t>
   </si>
+  <si>
+    <t>Pass/Fail (22/10/2019)</t>
+  </si>
+  <si>
+    <t>Timetable</t>
+  </si>
+  <si>
+    <t>Check if successful bid gets added to timetable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add bid for IS101 and IS102 </t>
+  </si>
+  <si>
+    <t>Add bid for IS101 and IS102</t>
+  </si>
+  <si>
+    <t>Both bids are supposed to be added to the timetable</t>
+  </si>
+  <si>
+    <t>Only the bid for IS102 is added to the timetable. IS101 is not reflected on the timetable.</t>
+  </si>
+  <si>
+    <t>Bootstrapping</t>
+  </si>
+  <si>
+    <t>Round 2 bids should be cleared</t>
+  </si>
+  <si>
+    <t>Round 2 bids are cleared</t>
+  </si>
+  <si>
+    <t>Re-bootstrap to round 1</t>
+  </si>
+  <si>
+    <t>Round 2 bids should be cleared when system is re-bootstrapped to round 1</t>
+  </si>
+  <si>
+    <t>Dropping of section is done when a round is active. i.e. success bids from round 2 are final and cannot be dropped</t>
+  </si>
+  <si>
+    <t>Drop Section</t>
+  </si>
+  <si>
+    <t>Drop section when round is not active</t>
+  </si>
+  <si>
+    <t>Unable to drop section when round is not active</t>
+  </si>
+  <si>
+    <t>Dropping section is possible when round is not active</t>
+  </si>
+  <si>
+    <t>Minimum bid</t>
+  </si>
+  <si>
+    <t>The minimum bid value should remain the same when there are still unfilled vacancies in the section</t>
+  </si>
+  <si>
+    <t>When there are two vacancies, if one person bids $10, the second person is also allowed to bid $10</t>
+  </si>
+  <si>
+    <t>In a section with 2 vacancies, second person enters minimum bid of $10</t>
+  </si>
+  <si>
+    <t>Second person should be allowed to bid for $10 (as minimum bid)</t>
+  </si>
+  <si>
+    <t>Second person is not allowed to bid for $10 (minimum bid raises to $11)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2625,31 +2695,43 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -2750,7 +2832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2781,6 +2863,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3001,8 +3084,8 @@
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4476,7 +4559,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4617,8 +4700,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4713,7 +4796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03581E9B-5434-EB41-ABEB-2F66EF42EF28}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -5673,8 +5756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED20DAA-AFB2-5240-A261-8BB8E5918D09}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="76" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6385,10 +6468,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA8D5A-5628-41F0-8C3D-F219DADB62EC}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6398,9 +6481,10 @@
     <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
     <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6426,7 +6510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -6435,8 +6519,11 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="12" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6462,7 +6549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6488,7 +6575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -6514,7 +6601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -6540,7 +6627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="70" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -6566,7 +6653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -6592,7 +6679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6618,7 +6705,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="42" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6644,7 +6731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6670,7 +6757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6696,7 +6783,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -6706,7 +6793,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -6716,7 +6803,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -6726,7 +6813,685 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7DF693-2CB7-4466-BEA5-4F1CA05A97CD}">
+  <dimension ref="A1:I56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="12" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="56" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>

</xml_diff>